<commit_message>
one pager render works
</commit_message>
<xml_diff>
--- a/input_template.xlsx
+++ b/input_template.xlsx
@@ -27,24 +27,24 @@
     <definedName name="Aantal_dagen">Algemeen!$B$19</definedName>
     <definedName name="Voorschot_borg">Algemeen!$B$22</definedName>
     <definedName name="Voorschot_GWE">Algemeen!$B$23</definedName>
-    <definedName name="Voorschot_schoonmaak">Algemeen!$B$24</definedName>
     <definedName name="Overige_voorschotten">Algemeen!$B$25</definedName>
-    <definedName name="Schoonmaak_pakket">Algemeen!$B$28</definedName>
-    <definedName name="Inbegrepen_uren">Algemeen!$B$29</definedName>
-    <definedName name="Uurtarief_schoonmaak">Algemeen!$B$30</definedName>
-    <definedName name="Meterbeheerder">Algemeen!$B$31</definedName>
-    <definedName name="Energie_leverancier">Algemeen!$B$32</definedName>
-    <definedName name="Contractnummer">Algemeen!$B$33</definedName>
-    <definedName name="RR_Klantnummer">Algemeen!$B$36</definedName>
-    <definedName name="RR_Folder_link">Algemeen!$B$37</definedName>
-    <definedName name="RR_Projectleider">Algemeen!$B$38</definedName>
-    <definedName name="RR_Inspecteur">Algemeen!$B$39</definedName>
-    <definedName name="RR_Factuurnummer">Algemeen!$B$40</definedName>
-    <definedName name="Borg_gebruikt">Algemeen!$B$43</definedName>
-    <definedName name="Borg_terug">Algemeen!$B$44</definedName>
-    <definedName name="Restschade">Algemeen!$B$45</definedName>
-    <definedName name="GWE_meer_minder">Algemeen!$B$46</definedName>
-    <definedName name="Totaal_eindafrekening">Algemeen!$B$47</definedName>
+    <definedName name="Schoonmaak_pakket_type">Algemeen!$B$28</definedName>
+    <definedName name="Voorschot_schoonmaak">Algemeen!$B$29</definedName>
+    <definedName name="Inbegrepen_uren">Algemeen!$B$30</definedName>
+    <definedName name="Uurtarief_schoonmaak">Algemeen!$B$31</definedName>
+    <definedName name="Meterbeheerder">Algemeen!$B$32</definedName>
+    <definedName name="Energie_leverancier">Algemeen!$B$33</definedName>
+    <definedName name="Contractnummer">Algemeen!$B$34</definedName>
+    <definedName name="RR_Klantnummer">Algemeen!$B$37</definedName>
+    <definedName name="RR_Folder_link">Algemeen!$B$38</definedName>
+    <definedName name="RR_Projectleider">Algemeen!$B$39</definedName>
+    <definedName name="RR_Inspecteur">Algemeen!$B$40</definedName>
+    <definedName name="RR_Factuurnummer">Algemeen!$B$41</definedName>
+    <definedName name="Borg_gebruikt">Algemeen!$B$44</definedName>
+    <definedName name="Borg_terug">Algemeen!$B$45</definedName>
+    <definedName name="Restschade">Algemeen!$B$46</definedName>
+    <definedName name="GWE_meer_minder">Algemeen!$B$47</definedName>
+    <definedName name="Totaal_eindafrekening">Algemeen!$B$48</definedName>
     <definedName name="KWh_begin">GWE_Detail!$B$4</definedName>
     <definedName name="KWh_eind">GWE_Detail!$B$5</definedName>
     <definedName name="KWh_verbruik">GWE_Detail!$B$6</definedName>
@@ -257,13 +257,13 @@
       <protection locked="0" hidden="0"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <protection locked="0" hidden="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <protection locked="0" hidden="0"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <protection locked="0" hidden="0"/>
     </xf>
@@ -696,7 +696,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -905,12 +905,8 @@
       <c r="C23" s="2" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="4" t="inlineStr">
-        <is>
-          <t>Voorschot Schoonmaak *</t>
-        </is>
-      </c>
-      <c r="B24" s="9" t="n"/>
+      <c r="A24" s="2" t="n"/>
+      <c r="B24" s="2" t="n"/>
       <c r="C24" s="2" t="n"/>
     </row>
     <row r="25">
@@ -944,17 +940,21 @@
           <t>Schoonmaak Pakket *</t>
         </is>
       </c>
-      <c r="B28" s="5" t="n"/>
+      <c r="B28" s="5" t="inlineStr">
+        <is>
+          <t>Basis Schoonmaak</t>
+        </is>
+      </c>
       <c r="C28" s="2" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="4" t="inlineStr">
         <is>
-          <t>Inbegrepen Uren (automatisch)</t>
-        </is>
-      </c>
-      <c r="B29" s="8">
-        <f>IF(B28="5_uur",5,IF(B28="7_uur",7,""))</f>
+          <t>Voorschot Schoonmaak (automatisch)</t>
+        </is>
+      </c>
+      <c r="B29" s="11">
+        <f>IF(B28="Basis Schoonmaak",250,IF(B28="Intensief Schoonmaak",350,0))</f>
         <v/>
       </c>
       <c r="C29" s="2" t="n"/>
@@ -962,27 +962,30 @@
     <row r="30">
       <c r="A30" s="4" t="inlineStr">
         <is>
-          <t>Uurtarief Schoonmaak *</t>
-        </is>
-      </c>
-      <c r="B30" s="9" t="n">
-        <v>50</v>
+          <t>Inbegrepen Uren (automatisch)</t>
+        </is>
+      </c>
+      <c r="B30" s="8">
+        <f>IF(B28="Basis Schoonmaak",5,IF(B28="Intensief Schoonmaak",7,0))</f>
+        <v/>
       </c>
       <c r="C30" s="2" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="4" t="inlineStr">
         <is>
-          <t>Meterbeheerder</t>
-        </is>
-      </c>
-      <c r="B31" s="6" t="n"/>
+          <t>Uurtarief Schoonmaak *</t>
+        </is>
+      </c>
+      <c r="B31" s="9" t="n">
+        <v>50</v>
+      </c>
       <c r="C31" s="2" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="4" t="inlineStr">
         <is>
-          <t>Energie Leverancier</t>
+          <t>Meterbeheerder</t>
         </is>
       </c>
       <c r="B32" s="6" t="n"/>
@@ -991,39 +994,39 @@
     <row r="33">
       <c r="A33" s="4" t="inlineStr">
         <is>
-          <t>Contractnummer</t>
+          <t>Energie Leverancier</t>
         </is>
       </c>
       <c r="B33" s="6" t="n"/>
       <c r="C33" s="2" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" s="2" t="n"/>
-      <c r="B34" s="2" t="n"/>
+      <c r="A34" s="4" t="inlineStr">
+        <is>
+          <t>Contractnummer</t>
+        </is>
+      </c>
+      <c r="B34" s="6" t="n"/>
       <c r="C34" s="2" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="3" t="inlineStr">
-        <is>
-          <t>INTERNE RYANRENT GEGEVENS</t>
-        </is>
-      </c>
+      <c r="A35" s="2" t="n"/>
       <c r="B35" s="2" t="n"/>
       <c r="C35" s="2" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="4" t="inlineStr">
-        <is>
-          <t>RR Klantnummer</t>
-        </is>
-      </c>
-      <c r="B36" s="6" t="n"/>
+      <c r="A36" s="3" t="inlineStr">
+        <is>
+          <t>INTERNE RYANRENT GEGEVENS</t>
+        </is>
+      </c>
+      <c r="B36" s="2" t="n"/>
       <c r="C36" s="2" t="n"/>
     </row>
     <row r="37">
       <c r="A37" s="4" t="inlineStr">
         <is>
-          <t>RR Folder Link</t>
+          <t>RR Klantnummer</t>
         </is>
       </c>
       <c r="B37" s="6" t="n"/>
@@ -1032,7 +1035,7 @@
     <row r="38">
       <c r="A38" s="4" t="inlineStr">
         <is>
-          <t>RR Projectleider</t>
+          <t>RR Folder Link</t>
         </is>
       </c>
       <c r="B38" s="6" t="n"/>
@@ -1041,7 +1044,7 @@
     <row r="39">
       <c r="A39" s="4" t="inlineStr">
         <is>
-          <t>RR Inspecteur</t>
+          <t>RR Projectleider</t>
         </is>
       </c>
       <c r="B39" s="6" t="n"/>
@@ -1050,50 +1053,47 @@
     <row r="40">
       <c r="A40" s="4" t="inlineStr">
         <is>
-          <t>RR Factuurnummer</t>
+          <t>RR Inspecteur</t>
         </is>
       </c>
       <c r="B40" s="6" t="n"/>
       <c r="C40" s="2" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="2" t="n"/>
-      <c r="B41" s="2" t="n"/>
+      <c r="A41" s="4" t="inlineStr">
+        <is>
+          <t>RR Factuurnummer</t>
+        </is>
+      </c>
+      <c r="B41" s="6" t="n"/>
       <c r="C41" s="2" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="11" t="inlineStr">
+      <c r="A42" s="2" t="n"/>
+      <c r="B42" s="2" t="n"/>
+      <c r="C42" s="2" t="n"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="12" t="inlineStr">
         <is>
           <t>BEREKENDE VELDEN (automatisch berekend)</t>
         </is>
       </c>
-      <c r="B42" s="2" t="n"/>
-      <c r="C42" s="12" t="inlineStr">
+      <c r="B43" s="2" t="n"/>
+      <c r="C43" s="13" t="inlineStr">
         <is>
           <t>← Live preview (beveiligd)</t>
         </is>
       </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="4" t="inlineStr">
-        <is>
-          <t>Borg Gebruikt (automatisch)</t>
-        </is>
-      </c>
-      <c r="B43" s="13">
-        <f>Schade!Schade_totaal_incl</f>
-        <v/>
-      </c>
-      <c r="C43" s="2" t="n"/>
     </row>
     <row r="44">
       <c r="A44" s="4" t="inlineStr">
         <is>
-          <t>Borg Terug (automatisch)</t>
-        </is>
-      </c>
-      <c r="B44" s="13">
-        <f>IF(Borg_gebruikt="","",Voorschot_borg-Borg_gebruikt)</f>
+          <t>Borg Gebruikt (automatisch)</t>
+        </is>
+      </c>
+      <c r="B44" s="11">
+        <f>Schade!Schade_totaal_incl</f>
         <v/>
       </c>
       <c r="C44" s="2" t="n"/>
@@ -1101,11 +1101,11 @@
     <row r="45">
       <c r="A45" s="4" t="inlineStr">
         <is>
-          <t>Restschade (automatisch)</t>
-        </is>
-      </c>
-      <c r="B45" s="13">
-        <f>IF(Borg_gebruikt="","",MAX(0,Borg_gebruikt-Voorschot_borg))</f>
+          <t>Borg Terug (automatisch)</t>
+        </is>
+      </c>
+      <c r="B45" s="11">
+        <f>IF(Borg_gebruikt="","",Voorschot_borg-Borg_gebruikt)</f>
         <v/>
       </c>
       <c r="C45" s="2" t="n"/>
@@ -1113,42 +1113,54 @@
     <row r="46">
       <c r="A46" s="4" t="inlineStr">
         <is>
+          <t>Restschade (automatisch)</t>
+        </is>
+      </c>
+      <c r="B46" s="11">
+        <f>IF(Borg_gebruikt="","",MAX(0,Borg_gebruikt-Voorschot_borg))</f>
+        <v/>
+      </c>
+      <c r="C46" s="2" t="n"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="4" t="inlineStr">
+        <is>
           <t>GWE Meer/Minder (automatisch)</t>
         </is>
       </c>
-      <c r="B46" s="13">
+      <c r="B47" s="11">
         <f>IF(GWE_Detail!GWE_totaal_incl="","",Voorschot_GWE-GWE_Detail!GWE_totaal_incl)</f>
         <v/>
       </c>
-      <c r="C46" s="2" t="n"/>
-    </row>
-    <row r="47">
-      <c r="A47" s="14" t="inlineStr">
+      <c r="C47" s="2" t="n"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="14" t="inlineStr">
         <is>
           <t>Totaal Eindafrekening (automatisch)</t>
         </is>
       </c>
-      <c r="B47" s="15">
+      <c r="B48" s="15">
         <f>IF(OR(Borg_terug="",GWE_meer_minder="",Schoonmaak!Extra_schoonmaak_bedrag=""),"",Borg_terug+GWE_meer_minder-Schoonmaak!Extra_schoonmaak_bedrag)</f>
         <v/>
       </c>
-      <c r="C47" s="2" t="n"/>
+      <c r="C48" s="2" t="n"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1"/>
   <mergeCells count="8">
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A36:B36"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A35:B35"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation sqref="B28" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Ongeldige invoer" error="Kies 5_uur of 7_uur" type="list">
-      <formula1>"5_uur,7_uur"</formula1>
+    <dataValidation sqref="B28" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Ongeldige invoer" error="Kies Basis Schoonmaak of Intensief Schoonmaak" type="list">
+      <formula1>"Basis Schoonmaak,Intensief Schoonmaak"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1504,7 +1516,7 @@
       <c r="D34" s="2" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="11" t="inlineStr">
+      <c r="A35" s="12" t="inlineStr">
         <is>
           <t>TOTALEN (automatisch berekend)</t>
         </is>
@@ -1519,7 +1531,7 @@
           <t>Totaal excl. BTW (automatisch)</t>
         </is>
       </c>
-      <c r="B36" s="13">
+      <c r="B36" s="11">
         <f>SUM(D14:D34)</f>
         <v/>
       </c>
@@ -1532,7 +1544,7 @@
           <t>BTW 21% (automatisch)</t>
         </is>
       </c>
-      <c r="B37" s="13">
+      <c r="B37" s="11">
         <f>IF(B36="","",B36*0.21)</f>
         <v/>
       </c>
@@ -1607,7 +1619,7 @@
         </is>
       </c>
       <c r="B4" s="34">
-        <f>Algemeen!Schoonmaak_pakket</f>
+        <f>Algemeen!Schoonmaak_pakket_type</f>
         <v/>
       </c>
     </row>
@@ -1618,7 +1630,7 @@
         </is>
       </c>
       <c r="B5" s="8">
-        <f>IF(B4="5_uur",5,IF(B4="7_uur",7,""))</f>
+        <f>IF(B4="Basis Schoonmaak",5,IF(B4="Intensief Schoonmaak",7,0))</f>
         <v/>
       </c>
     </row>
@@ -1737,7 +1749,7 @@
       <c r="A6" s="6" t="n"/>
       <c r="B6" s="42" t="n"/>
       <c r="C6" s="28" t="n"/>
-      <c r="D6" s="13">
+      <c r="D6" s="11">
         <f>IF(AND(B6&lt;&gt;"",C6&lt;&gt;""),B6*C6,"")</f>
         <v/>
       </c>
@@ -1746,7 +1758,7 @@
       <c r="A7" s="6" t="n"/>
       <c r="B7" s="42" t="n"/>
       <c r="C7" s="28" t="n"/>
-      <c r="D7" s="13">
+      <c r="D7" s="11">
         <f>IF(AND(B7&lt;&gt;"",C7&lt;&gt;""),B7*C7,"")</f>
         <v/>
       </c>
@@ -1755,7 +1767,7 @@
       <c r="A8" s="6" t="n"/>
       <c r="B8" s="42" t="n"/>
       <c r="C8" s="28" t="n"/>
-      <c r="D8" s="13">
+      <c r="D8" s="11">
         <f>IF(AND(B8&lt;&gt;"",C8&lt;&gt;""),B8*C8,"")</f>
         <v/>
       </c>
@@ -1764,7 +1776,7 @@
       <c r="A9" s="6" t="n"/>
       <c r="B9" s="42" t="n"/>
       <c r="C9" s="28" t="n"/>
-      <c r="D9" s="13">
+      <c r="D9" s="11">
         <f>IF(AND(B9&lt;&gt;"",C9&lt;&gt;""),B9*C9,"")</f>
         <v/>
       </c>
@@ -1773,7 +1785,7 @@
       <c r="A10" s="6" t="n"/>
       <c r="B10" s="42" t="n"/>
       <c r="C10" s="28" t="n"/>
-      <c r="D10" s="13">
+      <c r="D10" s="11">
         <f>IF(AND(B10&lt;&gt;"",C10&lt;&gt;""),B10*C10,"")</f>
         <v/>
       </c>
@@ -1782,7 +1794,7 @@
       <c r="A11" s="6" t="n"/>
       <c r="B11" s="42" t="n"/>
       <c r="C11" s="28" t="n"/>
-      <c r="D11" s="13">
+      <c r="D11" s="11">
         <f>IF(AND(B11&lt;&gt;"",C11&lt;&gt;""),B11*C11,"")</f>
         <v/>
       </c>
@@ -1791,7 +1803,7 @@
       <c r="A12" s="6" t="n"/>
       <c r="B12" s="42" t="n"/>
       <c r="C12" s="28" t="n"/>
-      <c r="D12" s="13">
+      <c r="D12" s="11">
         <f>IF(AND(B12&lt;&gt;"",C12&lt;&gt;""),B12*C12,"")</f>
         <v/>
       </c>
@@ -1800,7 +1812,7 @@
       <c r="A13" s="6" t="n"/>
       <c r="B13" s="42" t="n"/>
       <c r="C13" s="28" t="n"/>
-      <c r="D13" s="13">
+      <c r="D13" s="11">
         <f>IF(AND(B13&lt;&gt;"",C13&lt;&gt;""),B13*C13,"")</f>
         <v/>
       </c>
@@ -1809,7 +1821,7 @@
       <c r="A14" s="6" t="n"/>
       <c r="B14" s="42" t="n"/>
       <c r="C14" s="28" t="n"/>
-      <c r="D14" s="13">
+      <c r="D14" s="11">
         <f>IF(AND(B14&lt;&gt;"",C14&lt;&gt;""),B14*C14,"")</f>
         <v/>
       </c>
@@ -1818,7 +1830,7 @@
       <c r="A15" s="6" t="n"/>
       <c r="B15" s="42" t="n"/>
       <c r="C15" s="28" t="n"/>
-      <c r="D15" s="13">
+      <c r="D15" s="11">
         <f>IF(AND(B15&lt;&gt;"",C15&lt;&gt;""),B15*C15,"")</f>
         <v/>
       </c>
@@ -1827,7 +1839,7 @@
       <c r="A16" s="6" t="n"/>
       <c r="B16" s="42" t="n"/>
       <c r="C16" s="28" t="n"/>
-      <c r="D16" s="13">
+      <c r="D16" s="11">
         <f>IF(AND(B16&lt;&gt;"",C16&lt;&gt;""),B16*C16,"")</f>
         <v/>
       </c>
@@ -1836,7 +1848,7 @@
       <c r="A17" s="6" t="n"/>
       <c r="B17" s="42" t="n"/>
       <c r="C17" s="28" t="n"/>
-      <c r="D17" s="13">
+      <c r="D17" s="11">
         <f>IF(AND(B17&lt;&gt;"",C17&lt;&gt;""),B17*C17,"")</f>
         <v/>
       </c>
@@ -1845,7 +1857,7 @@
       <c r="A18" s="6" t="n"/>
       <c r="B18" s="42" t="n"/>
       <c r="C18" s="28" t="n"/>
-      <c r="D18" s="13">
+      <c r="D18" s="11">
         <f>IF(AND(B18&lt;&gt;"",C18&lt;&gt;""),B18*C18,"")</f>
         <v/>
       </c>
@@ -1854,7 +1866,7 @@
       <c r="A19" s="6" t="n"/>
       <c r="B19" s="42" t="n"/>
       <c r="C19" s="28" t="n"/>
-      <c r="D19" s="13">
+      <c r="D19" s="11">
         <f>IF(AND(B19&lt;&gt;"",C19&lt;&gt;""),B19*C19,"")</f>
         <v/>
       </c>
@@ -1863,7 +1875,7 @@
       <c r="A20" s="6" t="n"/>
       <c r="B20" s="42" t="n"/>
       <c r="C20" s="28" t="n"/>
-      <c r="D20" s="13">
+      <c r="D20" s="11">
         <f>IF(AND(B20&lt;&gt;"",C20&lt;&gt;""),B20*C20,"")</f>
         <v/>
       </c>
@@ -1872,7 +1884,7 @@
       <c r="A21" s="6" t="n"/>
       <c r="B21" s="42" t="n"/>
       <c r="C21" s="28" t="n"/>
-      <c r="D21" s="13">
+      <c r="D21" s="11">
         <f>IF(AND(B21&lt;&gt;"",C21&lt;&gt;""),B21*C21,"")</f>
         <v/>
       </c>
@@ -1881,7 +1893,7 @@
       <c r="A22" s="6" t="n"/>
       <c r="B22" s="42" t="n"/>
       <c r="C22" s="28" t="n"/>
-      <c r="D22" s="13">
+      <c r="D22" s="11">
         <f>IF(AND(B22&lt;&gt;"",C22&lt;&gt;""),B22*C22,"")</f>
         <v/>
       </c>
@@ -1890,7 +1902,7 @@
       <c r="A23" s="6" t="n"/>
       <c r="B23" s="42" t="n"/>
       <c r="C23" s="28" t="n"/>
-      <c r="D23" s="13">
+      <c r="D23" s="11">
         <f>IF(AND(B23&lt;&gt;"",C23&lt;&gt;""),B23*C23,"")</f>
         <v/>
       </c>
@@ -1899,7 +1911,7 @@
       <c r="A24" s="6" t="n"/>
       <c r="B24" s="42" t="n"/>
       <c r="C24" s="28" t="n"/>
-      <c r="D24" s="13">
+      <c r="D24" s="11">
         <f>IF(AND(B24&lt;&gt;"",C24&lt;&gt;""),B24*C24,"")</f>
         <v/>
       </c>
@@ -1908,7 +1920,7 @@
       <c r="A25" s="6" t="n"/>
       <c r="B25" s="42" t="n"/>
       <c r="C25" s="28" t="n"/>
-      <c r="D25" s="13">
+      <c r="D25" s="11">
         <f>IF(AND(B25&lt;&gt;"",C25&lt;&gt;""),B25*C25,"")</f>
         <v/>
       </c>
@@ -1917,7 +1929,7 @@
       <c r="A26" s="6" t="n"/>
       <c r="B26" s="42" t="n"/>
       <c r="C26" s="28" t="n"/>
-      <c r="D26" s="13">
+      <c r="D26" s="11">
         <f>IF(AND(B26&lt;&gt;"",C26&lt;&gt;""),B26*C26,"")</f>
         <v/>
       </c>
@@ -1926,7 +1938,7 @@
       <c r="A27" s="6" t="n"/>
       <c r="B27" s="42" t="n"/>
       <c r="C27" s="28" t="n"/>
-      <c r="D27" s="13">
+      <c r="D27" s="11">
         <f>IF(AND(B27&lt;&gt;"",C27&lt;&gt;""),B27*C27,"")</f>
         <v/>
       </c>
@@ -1935,7 +1947,7 @@
       <c r="A28" s="6" t="n"/>
       <c r="B28" s="42" t="n"/>
       <c r="C28" s="28" t="n"/>
-      <c r="D28" s="13">
+      <c r="D28" s="11">
         <f>IF(AND(B28&lt;&gt;"",C28&lt;&gt;""),B28*C28,"")</f>
         <v/>
       </c>
@@ -1944,7 +1956,7 @@
       <c r="A29" s="6" t="n"/>
       <c r="B29" s="42" t="n"/>
       <c r="C29" s="28" t="n"/>
-      <c r="D29" s="13">
+      <c r="D29" s="11">
         <f>IF(AND(B29&lt;&gt;"",C29&lt;&gt;""),B29*C29,"")</f>
         <v/>
       </c>
@@ -1953,7 +1965,7 @@
       <c r="A30" s="6" t="n"/>
       <c r="B30" s="42" t="n"/>
       <c r="C30" s="28" t="n"/>
-      <c r="D30" s="13">
+      <c r="D30" s="11">
         <f>IF(AND(B30&lt;&gt;"",C30&lt;&gt;""),B30*C30,"")</f>
         <v/>
       </c>
@@ -1962,7 +1974,7 @@
       <c r="A31" s="6" t="n"/>
       <c r="B31" s="42" t="n"/>
       <c r="C31" s="28" t="n"/>
-      <c r="D31" s="13">
+      <c r="D31" s="11">
         <f>IF(AND(B31&lt;&gt;"",C31&lt;&gt;""),B31*C31,"")</f>
         <v/>
       </c>
@@ -1971,7 +1983,7 @@
       <c r="A32" s="6" t="n"/>
       <c r="B32" s="42" t="n"/>
       <c r="C32" s="28" t="n"/>
-      <c r="D32" s="13">
+      <c r="D32" s="11">
         <f>IF(AND(B32&lt;&gt;"",C32&lt;&gt;""),B32*C32,"")</f>
         <v/>
       </c>
@@ -1980,7 +1992,7 @@
       <c r="A33" s="6" t="n"/>
       <c r="B33" s="42" t="n"/>
       <c r="C33" s="28" t="n"/>
-      <c r="D33" s="13">
+      <c r="D33" s="11">
         <f>IF(AND(B33&lt;&gt;"",C33&lt;&gt;""),B33*C33,"")</f>
         <v/>
       </c>
@@ -1989,7 +2001,7 @@
       <c r="A34" s="6" t="n"/>
       <c r="B34" s="42" t="n"/>
       <c r="C34" s="28" t="n"/>
-      <c r="D34" s="13">
+      <c r="D34" s="11">
         <f>IF(AND(B34&lt;&gt;"",C34&lt;&gt;""),B34*C34,"")</f>
         <v/>
       </c>
@@ -1998,7 +2010,7 @@
       <c r="A35" s="6" t="n"/>
       <c r="B35" s="42" t="n"/>
       <c r="C35" s="28" t="n"/>
-      <c r="D35" s="13">
+      <c r="D35" s="11">
         <f>IF(AND(B35&lt;&gt;"",C35&lt;&gt;""),B35*C35,"")</f>
         <v/>
       </c>
@@ -2007,7 +2019,7 @@
       <c r="A36" s="6" t="n"/>
       <c r="B36" s="42" t="n"/>
       <c r="C36" s="28" t="n"/>
-      <c r="D36" s="13">
+      <c r="D36" s="11">
         <f>IF(AND(B36&lt;&gt;"",C36&lt;&gt;""),B36*C36,"")</f>
         <v/>
       </c>
@@ -2016,7 +2028,7 @@
       <c r="A37" s="6" t="n"/>
       <c r="B37" s="42" t="n"/>
       <c r="C37" s="28" t="n"/>
-      <c r="D37" s="13">
+      <c r="D37" s="11">
         <f>IF(AND(B37&lt;&gt;"",C37&lt;&gt;""),B37*C37,"")</f>
         <v/>
       </c>
@@ -2025,7 +2037,7 @@
       <c r="A38" s="6" t="n"/>
       <c r="B38" s="42" t="n"/>
       <c r="C38" s="28" t="n"/>
-      <c r="D38" s="13">
+      <c r="D38" s="11">
         <f>IF(AND(B38&lt;&gt;"",C38&lt;&gt;""),B38*C38,"")</f>
         <v/>
       </c>
@@ -2034,7 +2046,7 @@
       <c r="A39" s="6" t="n"/>
       <c r="B39" s="42" t="n"/>
       <c r="C39" s="28" t="n"/>
-      <c r="D39" s="13">
+      <c r="D39" s="11">
         <f>IF(AND(B39&lt;&gt;"",C39&lt;&gt;""),B39*C39,"")</f>
         <v/>
       </c>
@@ -2043,7 +2055,7 @@
       <c r="A40" s="6" t="n"/>
       <c r="B40" s="42" t="n"/>
       <c r="C40" s="28" t="n"/>
-      <c r="D40" s="13">
+      <c r="D40" s="11">
         <f>IF(AND(B40&lt;&gt;"",C40&lt;&gt;""),B40*C40,"")</f>
         <v/>
       </c>
@@ -2052,7 +2064,7 @@
       <c r="A41" s="6" t="n"/>
       <c r="B41" s="42" t="n"/>
       <c r="C41" s="28" t="n"/>
-      <c r="D41" s="13">
+      <c r="D41" s="11">
         <f>IF(AND(B41&lt;&gt;"",C41&lt;&gt;""),B41*C41,"")</f>
         <v/>
       </c>
@@ -2061,7 +2073,7 @@
       <c r="A42" s="6" t="n"/>
       <c r="B42" s="42" t="n"/>
       <c r="C42" s="28" t="n"/>
-      <c r="D42" s="13">
+      <c r="D42" s="11">
         <f>IF(AND(B42&lt;&gt;"",C42&lt;&gt;""),B42*C42,"")</f>
         <v/>
       </c>
@@ -2070,7 +2082,7 @@
       <c r="A43" s="6" t="n"/>
       <c r="B43" s="42" t="n"/>
       <c r="C43" s="28" t="n"/>
-      <c r="D43" s="13">
+      <c r="D43" s="11">
         <f>IF(AND(B43&lt;&gt;"",C43&lt;&gt;""),B43*C43,"")</f>
         <v/>
       </c>
@@ -2079,7 +2091,7 @@
       <c r="A44" s="6" t="n"/>
       <c r="B44" s="42" t="n"/>
       <c r="C44" s="28" t="n"/>
-      <c r="D44" s="13">
+      <c r="D44" s="11">
         <f>IF(AND(B44&lt;&gt;"",C44&lt;&gt;""),B44*C44,"")</f>
         <v/>
       </c>
@@ -2088,7 +2100,7 @@
       <c r="A45" s="6" t="n"/>
       <c r="B45" s="42" t="n"/>
       <c r="C45" s="28" t="n"/>
-      <c r="D45" s="13">
+      <c r="D45" s="11">
         <f>IF(AND(B45&lt;&gt;"",C45&lt;&gt;""),B45*C45,"")</f>
         <v/>
       </c>
@@ -2097,7 +2109,7 @@
       <c r="A46" s="6" t="n"/>
       <c r="B46" s="42" t="n"/>
       <c r="C46" s="28" t="n"/>
-      <c r="D46" s="13">
+      <c r="D46" s="11">
         <f>IF(AND(B46&lt;&gt;"",C46&lt;&gt;""),B46*C46,"")</f>
         <v/>
       </c>
@@ -2106,7 +2118,7 @@
       <c r="A47" s="6" t="n"/>
       <c r="B47" s="42" t="n"/>
       <c r="C47" s="28" t="n"/>
-      <c r="D47" s="13">
+      <c r="D47" s="11">
         <f>IF(AND(B47&lt;&gt;"",C47&lt;&gt;""),B47*C47,"")</f>
         <v/>
       </c>
@@ -2115,7 +2127,7 @@
       <c r="A48" s="6" t="n"/>
       <c r="B48" s="42" t="n"/>
       <c r="C48" s="28" t="n"/>
-      <c r="D48" s="13">
+      <c r="D48" s="11">
         <f>IF(AND(B48&lt;&gt;"",C48&lt;&gt;""),B48*C48,"")</f>
         <v/>
       </c>
@@ -2124,7 +2136,7 @@
       <c r="A49" s="6" t="n"/>
       <c r="B49" s="42" t="n"/>
       <c r="C49" s="28" t="n"/>
-      <c r="D49" s="13">
+      <c r="D49" s="11">
         <f>IF(AND(B49&lt;&gt;"",C49&lt;&gt;""),B49*C49,"")</f>
         <v/>
       </c>
@@ -2133,7 +2145,7 @@
       <c r="A50" s="6" t="n"/>
       <c r="B50" s="42" t="n"/>
       <c r="C50" s="28" t="n"/>
-      <c r="D50" s="13">
+      <c r="D50" s="11">
         <f>IF(AND(B50&lt;&gt;"",C50&lt;&gt;""),B50*C50,"")</f>
         <v/>
       </c>
@@ -2142,7 +2154,7 @@
       <c r="A51" s="6" t="n"/>
       <c r="B51" s="42" t="n"/>
       <c r="C51" s="28" t="n"/>
-      <c r="D51" s="13">
+      <c r="D51" s="11">
         <f>IF(AND(B51&lt;&gt;"",C51&lt;&gt;""),B51*C51,"")</f>
         <v/>
       </c>
@@ -2151,7 +2163,7 @@
       <c r="A52" s="6" t="n"/>
       <c r="B52" s="42" t="n"/>
       <c r="C52" s="28" t="n"/>
-      <c r="D52" s="13">
+      <c r="D52" s="11">
         <f>IF(AND(B52&lt;&gt;"",C52&lt;&gt;""),B52*C52,"")</f>
         <v/>
       </c>
@@ -2160,7 +2172,7 @@
       <c r="A53" s="6" t="n"/>
       <c r="B53" s="42" t="n"/>
       <c r="C53" s="28" t="n"/>
-      <c r="D53" s="13">
+      <c r="D53" s="11">
         <f>IF(AND(B53&lt;&gt;"",C53&lt;&gt;""),B53*C53,"")</f>
         <v/>
       </c>
@@ -2169,7 +2181,7 @@
       <c r="A54" s="6" t="n"/>
       <c r="B54" s="42" t="n"/>
       <c r="C54" s="28" t="n"/>
-      <c r="D54" s="13">
+      <c r="D54" s="11">
         <f>IF(AND(B54&lt;&gt;"",C54&lt;&gt;""),B54*C54,"")</f>
         <v/>
       </c>
@@ -2178,7 +2190,7 @@
       <c r="A55" s="6" t="n"/>
       <c r="B55" s="42" t="n"/>
       <c r="C55" s="28" t="n"/>
-      <c r="D55" s="13">
+      <c r="D55" s="11">
         <f>IF(AND(B55&lt;&gt;"",C55&lt;&gt;""),B55*C55,"")</f>
         <v/>
       </c>
@@ -2197,7 +2209,7 @@
           <t>Totaal Schade excl. BTW (automatisch)</t>
         </is>
       </c>
-      <c r="B58" s="13">
+      <c r="B58" s="11">
         <f>SUM(D6:D56)</f>
         <v/>
       </c>
@@ -2208,7 +2220,7 @@
           <t>BTW 21% (automatisch)</t>
         </is>
       </c>
-      <c r="B59" s="13">
+      <c r="B59" s="11">
         <f>IF(B58="","",B58*0.21)</f>
         <v/>
       </c>
@@ -2491,13 +2503,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDC0AA90-838E-4DA5-89AC-D898F3EEACF2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBBA84A9-397E-4E12-BFFB-0436634DA3D5}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFDE96B4-D630-40E7-ACFB-51B9D3C7AA8F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D15C3191-FDC9-4D92-8235-1C644D319F44}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FB02099-F4CC-41A8-91DF-8DBD6C334DAE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B23D0D3-845A-442C-9FFB-B1B751F2D85B}"/>
 </file>
</xml_diff>

<commit_message>
upgrades pushed through close
</commit_message>
<xml_diff>
--- a/input_template.xlsx
+++ b/input_template.xlsx
@@ -1,75 +1,74 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20280" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Algemeen" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GWE_Detail" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Schoonmaak" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Schade" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Algemeen" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="GWE_Detail" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Schoonmaak" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Schade" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="Klantnaam">Algemeen!$B$4</definedName>
-    <definedName name="Contactpersoon">Algemeen!$B$5</definedName>
-    <definedName name="Email">Algemeen!$B$6</definedName>
-    <definedName name="Telefoonnummer">Algemeen!$B$7</definedName>
-    <definedName name="Object_adres">Algemeen!$B$10</definedName>
-    <definedName name="Unit_nr">Algemeen!$B$11</definedName>
-    <definedName name="Postcode">Algemeen!$B$12</definedName>
-    <definedName name="Plaats">Algemeen!$B$13</definedName>
-    <definedName name="Object_ID">Algemeen!$B$14</definedName>
-    <definedName name="Incheck_datum">Algemeen!$B$17</definedName>
-    <definedName name="Uitcheck_datum">Algemeen!$B$18</definedName>
     <definedName name="Aantal_dagen">Algemeen!$B$19</definedName>
-    <definedName name="Voorschot_borg">Algemeen!$B$22</definedName>
-    <definedName name="Voorschot_GWE">Algemeen!$B$23</definedName>
-    <definedName name="Overige_voorschotten">Algemeen!$B$25</definedName>
-    <definedName name="Schoonmaak_pakket_type">Algemeen!$B$28</definedName>
-    <definedName name="Voorschot_schoonmaak">Algemeen!$B$29</definedName>
-    <definedName name="Inbegrepen_uren">Algemeen!$B$30</definedName>
-    <definedName name="Uurtarief_schoonmaak">Algemeen!$B$31</definedName>
-    <definedName name="Meterbeheerder">Algemeen!$B$32</definedName>
-    <definedName name="Energie_leverancier">Algemeen!$B$33</definedName>
-    <definedName name="Contractnummer">Algemeen!$B$34</definedName>
-    <definedName name="RR_Klantnummer">Algemeen!$B$37</definedName>
-    <definedName name="RR_Folder_link">Algemeen!$B$38</definedName>
-    <definedName name="RR_Projectleider">Algemeen!$B$39</definedName>
-    <definedName name="RR_Inspecteur">Algemeen!$B$40</definedName>
-    <definedName name="RR_Factuurnummer">Algemeen!$B$41</definedName>
     <definedName name="Borg_gebruikt">Algemeen!$B$44</definedName>
     <definedName name="Borg_terug">Algemeen!$B$45</definedName>
-    <definedName name="Restschade">Algemeen!$B$46</definedName>
+    <definedName name="Contactpersoon">Algemeen!$B$5</definedName>
+    <definedName name="Contractnummer">Algemeen!$B$34</definedName>
+    <definedName name="Email">Algemeen!$B$6</definedName>
+    <definedName name="Energie_leverancier">Algemeen!$B$33</definedName>
+    <definedName name="Extra_schoonmaak_bedrag">Schoonmaak!$B$9</definedName>
+    <definedName name="Extra_uren">Schoonmaak!$B$7</definedName>
+    <definedName name="Gas_begin">GWE_Detail!$B$7</definedName>
+    <definedName name="Gas_eind">GWE_Detail!$B$8</definedName>
+    <definedName name="Gas_verbruik">GWE_Detail!$B$9</definedName>
+    <definedName name="GWE_BTW">GWE_Detail!$B$37</definedName>
     <definedName name="GWE_meer_minder">Algemeen!$B$47</definedName>
-    <definedName name="Totaal_eindafrekening">Algemeen!$B$48</definedName>
+    <definedName name="GWE_totaal_excl">GWE_Detail!$B$36</definedName>
+    <definedName name="GWE_totaal_incl">GWE_Detail!$B$38</definedName>
+    <definedName name="Inbegrepen_uren">Algemeen!$B$30</definedName>
+    <definedName name="Incheck_datum">Algemeen!$B$17</definedName>
+    <definedName name="Klantnaam">Algemeen!$B$4</definedName>
     <definedName name="KWh_begin">GWE_Detail!$B$4</definedName>
     <definedName name="KWh_eind">GWE_Detail!$B$5</definedName>
     <definedName name="KWh_verbruik">GWE_Detail!$B$6</definedName>
-    <definedName name="Gas_begin">GWE_Detail!$B$7</definedName>
-    <definedName name="Gas_eind">GWE_Detail!$B$8</definedName>
-    <definedName name="Gas_verbruik">GWE_Detail!$B$9</definedName>
-    <definedName name="GWE_totaal_excl">GWE_Detail!$B$36</definedName>
-    <definedName name="GWE_BTW">GWE_Detail!$B$37</definedName>
-    <definedName name="GWE_totaal_incl">GWE_Detail!$B$38</definedName>
+    <definedName name="Meterbeheerder">Algemeen!$B$32</definedName>
+    <definedName name="Object_adres">Algemeen!$B$10</definedName>
+    <definedName name="Object_ID">Algemeen!$B$14</definedName>
+    <definedName name="Overige_voorschotten">Algemeen!$B$25</definedName>
+    <definedName name="Plaats">Algemeen!$B$13</definedName>
+    <definedName name="Postcode">Algemeen!$B$12</definedName>
+    <definedName name="Restschade">Algemeen!$B$46</definedName>
+    <definedName name="RR_Factuurnummer">Algemeen!$B$41</definedName>
+    <definedName name="RR_Folder_link">Algemeen!$B$38</definedName>
+    <definedName name="RR_Inspecteur">Algemeen!$B$40</definedName>
+    <definedName name="RR_Klantnummer">Algemeen!$B$37</definedName>
+    <definedName name="RR_Projectleider">Algemeen!$B$39</definedName>
+    <definedName name="Schade_BTW">Schade!$B$59</definedName>
+    <definedName name="Schade_totaal_excl">Schade!$B$58</definedName>
+    <definedName name="Schade_totaal_incl">Schade!$B$60</definedName>
+    <definedName name="Schoonmaak_pakket_type">Algemeen!$B$28</definedName>
+    <definedName name="Telefoonnummer">Algemeen!$B$7</definedName>
+    <definedName name="Totaal_eindafrekening">Algemeen!$B$48</definedName>
     <definedName name="Totaal_uren_gew">Schoonmaak!$B$6</definedName>
-    <definedName name="Extra_uren">Schoonmaak!$B$7</definedName>
-    <definedName name="Extra_schoonmaak_bedrag">Schoonmaak!$B$9</definedName>
-    <definedName name="Schade_totaal_excl">Schade!$B$58</definedName>
-    <definedName name="Schade_BTW">Schade!$B$59</definedName>
-    <definedName name="Schade_totaal_incl">Schade!$B$60</definedName>
+    <definedName name="Uitcheck_datum">Algemeen!$B$18</definedName>
+    <definedName name="Unit_nr">Algemeen!$B$11</definedName>
+    <definedName name="Uurtarief_schoonmaak">Algemeen!$B$31</definedName>
+    <definedName name="Voorschot_borg">Algemeen!$B$22</definedName>
+    <definedName name="Voorschot_GWE">Algemeen!$B$23</definedName>
+    <definedName name="Voorschot_schoonmaak">Algemeen!$B$29</definedName>
   </definedNames>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="DD-MM-YYYY"/>
-    <numFmt numFmtId="165" formatCode="€ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
+    <numFmt numFmtId="165" formatCode="\€\ #,##0.00"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -81,57 +80,72 @@
     </font>
     <font>
       <name val="Arial"/>
+      <family val="2"/>
       <b val="1"/>
-      <color rgb="00FFFFFF"/>
+      <color rgb="FFFFFFFF"/>
       <sz val="12"/>
     </font>
     <font>
       <name val="Arial"/>
+      <family val="2"/>
       <b val="1"/>
-      <color rgb="00FFFFFF"/>
+      <color rgb="FFFFFFFF"/>
       <sz val="11"/>
     </font>
     <font>
       <name val="Arial"/>
+      <family val="2"/>
       <sz val="10"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
       <i val="1"/>
-      <color rgb="00C0504D"/>
+      <color rgb="FFC0504D"/>
+      <sz val="11"/>
     </font>
     <font>
       <name val="Arial"/>
+      <family val="2"/>
       <b val="1"/>
       <sz val="11"/>
     </font>
     <font>
       <name val="Arial"/>
+      <family val="2"/>
       <i val="1"/>
       <sz val="9"/>
     </font>
     <font>
       <name val="Arial"/>
+      <family val="2"/>
       <b val="1"/>
-      <color rgb="00FFFFFF"/>
+      <color rgb="FFFFFFFF"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
+      <family val="2"/>
       <i val="1"/>
-      <color rgb="00666666"/>
+      <color rgb="FF666666"/>
       <sz val="9"/>
     </font>
     <font>
       <name val="Arial"/>
+      <family val="2"/>
       <b val="1"/>
       <sz val="10"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
       <i val="1"/>
-      <color rgb="00666666"/>
+      <color rgb="FF666666"/>
+      <sz val="11"/>
     </font>
     <font>
       <name val="Arial"/>
+      <family val="2"/>
       <i val="1"/>
       <sz val="10"/>
     </font>
@@ -145,66 +159,66 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="001F4E78"/>
-        <bgColor rgb="001F4E78"/>
+        <fgColor rgb="FF1F4E78"/>
+        <bgColor rgb="FF1F4E78"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="005B9BD5"/>
-        <bgColor rgb="005B9BD5"/>
+        <fgColor rgb="FF5B9BD5"/>
+        <bgColor rgb="FF5B9BD5"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFF2CC"/>
-        <bgColor rgb="00FFF2CC"/>
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00E7E6E6"/>
-        <bgColor rgb="00E7E6E6"/>
+        <fgColor rgb="FFE7E6E6"/>
+        <bgColor rgb="FFE7E6E6"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00C0504D"/>
-        <bgColor rgb="00C0504D"/>
+        <fgColor rgb="FFC0504D"/>
+        <bgColor rgb="FFC0504D"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0070AD47"/>
-        <bgColor rgb="0070AD47"/>
+        <fgColor rgb="FF70AD47"/>
+        <bgColor rgb="FF70AD47"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00A9D08E"/>
-        <bgColor rgb="00A9D08E"/>
+        <fgColor rgb="FFA9D08E"/>
+        <bgColor rgb="FFA9D08E"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00F2F2F2"/>
-        <bgColor rgb="00F2F2F2"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFC000"/>
-        <bgColor rgb="00FFC000"/>
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFFFC000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFD966"/>
-        <bgColor rgb="00FFD966"/>
+        <fgColor rgb="FFFFD966"/>
+        <bgColor rgb="FFFFD966"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -213,31 +227,86 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <protection locked="0" hidden="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -258,9 +327,6 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <protection locked="0" hidden="0"/>
     </xf>
@@ -268,13 +334,6 @@
       <protection locked="0" hidden="0"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="5" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="4" borderId="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <protection locked="0" hidden="0"/>
     </xf>
@@ -283,9 +342,6 @@
       <protection locked="0" hidden="0"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0" hidden="0"/>
@@ -305,10 +361,6 @@
       <protection locked="0" hidden="0"/>
     </xf>
     <xf numFmtId="165" fontId="9" fillId="5" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -317,22 +369,111 @@
     <xf numFmtId="2" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="10" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="2" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="5" borderId="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="9" borderId="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="9" borderId="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="5" borderId="2" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="4" borderId="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -692,462 +833,521 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <tabColor rgb="001F4E78"/>
+    <tabColor rgb="FF1F4E78"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col width="30" customWidth="1" min="1" max="1"/>
-    <col width="35" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" style="48" min="1" max="1"/>
+    <col width="35" customWidth="1" style="48" min="2" max="2"/>
+    <col width="20" customWidth="1" style="48" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1" ht="16" customHeight="1" s="48">
+      <c r="A1" s="36" t="inlineStr">
         <is>
           <t>RYANRENT EINDAFREKENING - BASISGEGEVENS</t>
         </is>
       </c>
-      <c r="B1" s="2" t="n"/>
-      <c r="C1" s="2" t="n"/>
+      <c r="B1" s="34" t="n"/>
+      <c r="C1" s="1" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n"/>
-      <c r="B2" s="2" t="n"/>
-      <c r="C2" s="2" t="n"/>
+      <c r="A2" s="1" t="n"/>
+      <c r="B2" s="1" t="n"/>
+      <c r="C2" s="1" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="inlineStr">
+      <c r="A3" s="33" t="inlineStr">
         <is>
           <t>KLANTGEGEVENS</t>
         </is>
       </c>
-      <c r="B3" s="2" t="n"/>
-      <c r="C3" s="2" t="n"/>
+      <c r="B3" s="34" t="n"/>
+      <c r="C3" s="1" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>Naam Klant *</t>
         </is>
       </c>
-      <c r="B4" s="5" t="n"/>
-      <c r="C4" s="2" t="n"/>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>Familie Janssen</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>Contactpersoon</t>
         </is>
       </c>
-      <c r="B5" s="6" t="n"/>
-      <c r="C5" s="2" t="n"/>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>Anna van RyanRent</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>Email *</t>
         </is>
       </c>
-      <c r="B6" s="5" t="n"/>
-      <c r="C6" s="2" t="n"/>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>m.janssen@email.nl</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>Telefoonnummer</t>
         </is>
       </c>
-      <c r="B7" s="6" t="n"/>
-      <c r="C7" s="2" t="n"/>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>06-11223344</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="n"/>
-      <c r="B8" s="2" t="n"/>
-      <c r="C8" s="2" t="n"/>
+      <c r="A8" s="1" t="n"/>
+      <c r="B8" s="1" t="n"/>
+      <c r="C8" s="1" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="inlineStr">
+      <c r="A9" s="33" t="inlineStr">
         <is>
           <t>OBJECTGEGEVENS</t>
         </is>
       </c>
-      <c r="B9" s="2" t="n"/>
-      <c r="C9" s="2" t="n"/>
+      <c r="B9" s="34" t="n"/>
+      <c r="C9" s="1" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="inlineStr">
+      <c r="A10" s="2" t="inlineStr">
         <is>
           <t>Adres Object *</t>
         </is>
       </c>
-      <c r="B10" s="5" t="n"/>
-      <c r="C10" s="2" t="n"/>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>Kustlaan 88B, 4321AB Zandvoort</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="inlineStr">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>Unit Nummer</t>
         </is>
       </c>
-      <c r="B11" s="6" t="n"/>
-      <c r="C11" s="2" t="n"/>
+      <c r="B11" s="4" t="inlineStr">
+        <is>
+          <t>88B</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="inlineStr">
+      <c r="A12" s="2" t="inlineStr">
         <is>
           <t>Postcode</t>
         </is>
       </c>
-      <c r="B12" s="6" t="n"/>
-      <c r="C12" s="2" t="n"/>
+      <c r="B12" s="4" t="inlineStr">
+        <is>
+          <t>4321AB</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="4" t="inlineStr">
+      <c r="A13" s="2" t="inlineStr">
         <is>
           <t>Plaats</t>
         </is>
       </c>
-      <c r="B13" s="6" t="n"/>
-      <c r="C13" s="2" t="n"/>
+      <c r="B13" s="4" t="inlineStr">
+        <is>
+          <t>Zandvoort</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="inlineStr">
+      <c r="A14" s="2" t="inlineStr">
         <is>
           <t>Object ID</t>
         </is>
       </c>
-      <c r="B14" s="6" t="n"/>
-      <c r="C14" s="2" t="n"/>
+      <c r="B14" s="4" t="inlineStr">
+        <is>
+          <t>RR-2024-088</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="n"/>
-      <c r="B15" s="2" t="n"/>
-      <c r="C15" s="2" t="n"/>
+      <c r="A15" s="1" t="n"/>
+      <c r="B15" s="1" t="n"/>
+      <c r="C15" s="1" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="inlineStr">
+      <c r="A16" s="33" t="inlineStr">
         <is>
           <t>VERBLIJFSPERIODE</t>
         </is>
       </c>
-      <c r="B16" s="2" t="n"/>
-      <c r="C16" s="2" t="n"/>
+      <c r="B16" s="34" t="n"/>
+      <c r="C16" s="1" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="4" t="inlineStr">
+      <c r="A17" s="2" t="inlineStr">
         <is>
           <t>Incheck Datum *</t>
         </is>
       </c>
-      <c r="B17" s="7" t="n"/>
-      <c r="C17" s="2" t="n"/>
+      <c r="B17" s="5" t="n">
+        <v>45853</v>
+      </c>
+      <c r="C17" s="1" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="inlineStr">
+      <c r="A18" s="2" t="inlineStr">
         <is>
           <t>Uitcheck Datum *</t>
         </is>
       </c>
-      <c r="B18" s="7" t="n"/>
-      <c r="C18" s="2" t="n"/>
+      <c r="B18" s="5" t="n">
+        <v>45867</v>
+      </c>
+      <c r="C18" s="1" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="4" t="inlineStr">
+      <c r="A19" s="2" t="inlineStr">
         <is>
           <t>Aantal Dagen (automatisch)</t>
         </is>
       </c>
-      <c r="B19" s="8">
-        <f>IF(AND(B17&lt;&gt;"",B18&lt;&gt;""),B18-B17,"")</f>
-        <v/>
-      </c>
-      <c r="C19" s="2" t="n"/>
+      <c r="B19" s="49" t="n">
+        <v>14</v>
+      </c>
+      <c r="C19" s="1" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="n"/>
-      <c r="B20" s="2" t="n"/>
-      <c r="C20" s="2" t="n"/>
+      <c r="A20" s="1" t="n"/>
+      <c r="B20" s="1" t="n"/>
+      <c r="C20" s="1" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="3" t="inlineStr">
+      <c r="A21" s="33" t="inlineStr">
         <is>
           <t>VOORSCHOTTEN</t>
         </is>
       </c>
-      <c r="B21" s="2" t="n"/>
-      <c r="C21" s="2" t="n"/>
+      <c r="B21" s="34" t="n"/>
+      <c r="C21" s="1" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="4" t="inlineStr">
+      <c r="A22" s="2" t="inlineStr">
         <is>
           <t>Voorschot Borg *</t>
         </is>
       </c>
-      <c r="B22" s="9" t="n"/>
-      <c r="C22" s="2" t="n"/>
+      <c r="B22" s="7" t="n">
+        <v>500</v>
+      </c>
+      <c r="C22" s="1" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="4" t="inlineStr">
+      <c r="A23" s="2" t="inlineStr">
         <is>
           <t>Voorschot GWE *</t>
         </is>
       </c>
-      <c r="B23" s="9" t="n"/>
-      <c r="C23" s="2" t="n"/>
+      <c r="B23" s="7" t="n">
+        <v>300</v>
+      </c>
+      <c r="C23" s="1" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="2" t="n"/>
-      <c r="B24" s="2" t="n"/>
-      <c r="C24" s="2" t="n"/>
+      <c r="A24" s="1" t="n"/>
+      <c r="B24" s="1" t="n"/>
+      <c r="C24" s="1" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="4" t="inlineStr">
+      <c r="A25" s="2" t="inlineStr">
         <is>
           <t>Overige Voorschotten</t>
         </is>
       </c>
-      <c r="B25" s="10" t="n">
+      <c r="B25" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="C25" s="2" t="n"/>
+      <c r="C25" s="1" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="2" t="n"/>
-      <c r="B26" s="2" t="n"/>
-      <c r="C26" s="2" t="n"/>
+      <c r="A26" s="1" t="n"/>
+      <c r="B26" s="1" t="n"/>
+      <c r="C26" s="1" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="3" t="inlineStr">
+      <c r="A27" s="33" t="inlineStr">
         <is>
           <t>CONTRACTGEGEVENS</t>
         </is>
       </c>
-      <c r="B27" s="2" t="n"/>
-      <c r="C27" s="2" t="n"/>
+      <c r="B27" s="34" t="n"/>
+      <c r="C27" s="1" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="4" t="inlineStr">
+      <c r="A28" s="2" t="inlineStr">
         <is>
           <t>Schoonmaak Pakket *</t>
         </is>
       </c>
-      <c r="B28" s="5" t="inlineStr">
-        <is>
-          <t>Basis Schoonmaak</t>
-        </is>
-      </c>
-      <c r="C28" s="2" t="n"/>
+      <c r="B28" s="3" t="inlineStr">
+        <is>
+          <t>al</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="4" t="inlineStr">
+      <c r="A29" s="2" t="inlineStr">
         <is>
           <t>Voorschot Schoonmaak (automatisch)</t>
         </is>
       </c>
-      <c r="B29" s="11">
-        <f>IF(B28="Basis Schoonmaak",250,IF(B28="Intensief Schoonmaak",350,0))</f>
-        <v/>
-      </c>
-      <c r="C29" s="2" t="n"/>
+      <c r="B29" s="50" t="n">
+        <v>250</v>
+      </c>
+      <c r="C29" s="1" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="4" t="inlineStr">
+      <c r="A30" s="2" t="inlineStr">
         <is>
           <t>Inbegrepen Uren (automatisch)</t>
         </is>
       </c>
-      <c r="B30" s="8">
-        <f>IF(B28="Basis Schoonmaak",5,IF(B28="Intensief Schoonmaak",7,0))</f>
-        <v/>
-      </c>
-      <c r="C30" s="2" t="n"/>
+      <c r="B30" s="49" t="n">
+        <v>5</v>
+      </c>
+      <c r="C30" s="1" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="4" t="inlineStr">
+      <c r="A31" s="2" t="inlineStr">
         <is>
           <t>Uurtarief Schoonmaak *</t>
         </is>
       </c>
-      <c r="B31" s="9" t="n">
+      <c r="B31" s="7" t="n">
         <v>50</v>
       </c>
-      <c r="C31" s="2" t="n"/>
+      <c r="C31" s="1" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="4" t="inlineStr">
+      <c r="A32" s="2" t="inlineStr">
         <is>
           <t>Meterbeheerder</t>
         </is>
       </c>
-      <c r="B32" s="6" t="n"/>
-      <c r="C32" s="2" t="n"/>
+      <c r="B32" s="4" t="inlineStr">
+        <is>
+          <t>Enexis</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="4" t="inlineStr">
+      <c r="A33" s="2" t="inlineStr">
         <is>
           <t>Energie Leverancier</t>
         </is>
       </c>
-      <c r="B33" s="6" t="n"/>
-      <c r="C33" s="2" t="n"/>
+      <c r="B33" s="4" t="inlineStr">
+        <is>
+          <t>Vattenfall</t>
+        </is>
+      </c>
+      <c r="C33" s="1" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" s="4" t="inlineStr">
+      <c r="A34" s="2" t="inlineStr">
         <is>
           <t>Contractnummer</t>
         </is>
       </c>
-      <c r="B34" s="6" t="n"/>
-      <c r="C34" s="2" t="n"/>
+      <c r="B34" s="4" t="n"/>
+      <c r="C34" s="1" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="2" t="n"/>
-      <c r="B35" s="2" t="n"/>
-      <c r="C35" s="2" t="n"/>
+      <c r="A35" s="1" t="n"/>
+      <c r="B35" s="1" t="n"/>
+      <c r="C35" s="1" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="3" t="inlineStr">
+      <c r="A36" s="33" t="inlineStr">
         <is>
           <t>INTERNE RYANRENT GEGEVENS</t>
         </is>
       </c>
-      <c r="B36" s="2" t="n"/>
-      <c r="C36" s="2" t="n"/>
+      <c r="B36" s="34" t="n"/>
+      <c r="C36" s="1" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="4" t="inlineStr">
+      <c r="A37" s="2" t="inlineStr">
         <is>
           <t>RR Klantnummer</t>
         </is>
       </c>
-      <c r="B37" s="6" t="n"/>
-      <c r="C37" s="2" t="n"/>
+      <c r="B37" s="4" t="inlineStr">
+        <is>
+          <t>KL-2025-088</t>
+        </is>
+      </c>
+      <c r="C37" s="1" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="4" t="inlineStr">
+      <c r="A38" s="2" t="inlineStr">
         <is>
           <t>RR Folder Link</t>
         </is>
       </c>
-      <c r="B38" s="6" t="n"/>
-      <c r="C38" s="2" t="n"/>
+      <c r="B38" s="4" t="n"/>
+      <c r="C38" s="1" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="4" t="inlineStr">
+      <c r="A39" s="2" t="inlineStr">
         <is>
           <t>RR Projectleider</t>
         </is>
       </c>
-      <c r="B39" s="6" t="n"/>
-      <c r="C39" s="2" t="n"/>
+      <c r="B39" s="4" t="inlineStr">
+        <is>
+          <t>Mark</t>
+        </is>
+      </c>
+      <c r="C39" s="1" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="4" t="inlineStr">
+      <c r="A40" s="2" t="inlineStr">
         <is>
           <t>RR Inspecteur</t>
         </is>
       </c>
-      <c r="B40" s="6" t="n"/>
-      <c r="C40" s="2" t="n"/>
+      <c r="B40" s="4" t="inlineStr">
+        <is>
+          <t>Anna</t>
+        </is>
+      </c>
+      <c r="C40" s="1" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="4" t="inlineStr">
+      <c r="A41" s="2" t="inlineStr">
         <is>
           <t>RR Factuurnummer</t>
         </is>
       </c>
-      <c r="B41" s="6" t="n"/>
-      <c r="C41" s="2" t="n"/>
+      <c r="B41" s="4" t="inlineStr">
+        <is>
+          <t>RR-2025-0042</t>
+        </is>
+      </c>
+      <c r="C41" s="1" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="2" t="n"/>
-      <c r="B42" s="2" t="n"/>
-      <c r="C42" s="2" t="n"/>
+      <c r="A42" s="1" t="n"/>
+      <c r="B42" s="1" t="n"/>
+      <c r="C42" s="1" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="12" t="inlineStr">
+      <c r="A43" s="35" t="inlineStr">
         <is>
           <t>BEREKENDE VELDEN (automatisch berekend)</t>
         </is>
       </c>
-      <c r="B43" s="2" t="n"/>
-      <c r="C43" s="13" t="inlineStr">
+      <c r="B43" s="34" t="n"/>
+      <c r="C43" s="10" t="inlineStr">
         <is>
           <t>← Live preview (beveiligd)</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="4" t="inlineStr">
+      <c r="A44" s="2" t="inlineStr">
         <is>
           <t>Borg Gebruikt (automatisch)</t>
         </is>
       </c>
-      <c r="B44" s="11">
-        <f>Schade!Schade_totaal_incl</f>
-        <v/>
-      </c>
-      <c r="C44" s="2" t="n"/>
+      <c r="B44" s="50" t="n">
+        <v>500</v>
+      </c>
+      <c r="C44" s="1" t="n"/>
     </row>
     <row r="45">
-      <c r="A45" s="4" t="inlineStr">
+      <c r="A45" s="2" t="inlineStr">
         <is>
           <t>Borg Terug (automatisch)</t>
         </is>
       </c>
-      <c r="B45" s="11">
-        <f>IF(Borg_gebruikt="","",Voorschot_borg-Borg_gebruikt)</f>
-        <v/>
-      </c>
-      <c r="C45" s="2" t="n"/>
+      <c r="B45" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="C45" s="1" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" s="4" t="inlineStr">
+      <c r="A46" s="2" t="inlineStr">
         <is>
           <t>Restschade (automatisch)</t>
         </is>
       </c>
-      <c r="B46" s="11">
-        <f>IF(Borg_gebruikt="","",MAX(0,Borg_gebruikt-Voorschot_borg))</f>
-        <v/>
-      </c>
-      <c r="C46" s="2" t="n"/>
+      <c r="B46" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="C46" s="1" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" s="4" t="inlineStr">
+      <c r="A47" s="2" t="inlineStr">
         <is>
           <t>GWE Meer/Minder (automatisch)</t>
         </is>
       </c>
-      <c r="B47" s="11">
-        <f>IF(GWE_Detail!GWE_totaal_incl="","",Voorschot_GWE-GWE_Detail!GWE_totaal_incl)</f>
-        <v/>
-      </c>
-      <c r="C47" s="2" t="n"/>
+      <c r="B47" s="50" t="n">
+        <v>-285.64</v>
+      </c>
+      <c r="C47" s="1" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" s="14" t="inlineStr">
+      <c r="A48" s="11" t="inlineStr">
         <is>
           <t>Totaal Eindafrekening (automatisch)</t>
         </is>
       </c>
-      <c r="B48" s="15">
-        <f>IF(OR(Borg_terug="",GWE_meer_minder="",Schoonmaak!Extra_schoonmaak_bedrag=""),"",Borg_terug+GWE_meer_minder-Schoonmaak!Extra_schoonmaak_bedrag)</f>
-        <v/>
-      </c>
-      <c r="C48" s="2" t="n"/>
+      <c r="B48" s="51" t="n">
+        <v>-410.64</v>
+      </c>
+      <c r="C48" s="1" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1"/>
   <mergeCells count="8">
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A16:B16"/>
@@ -1170,7 +1370,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <tabColor rgb="0070AD47"/>
+    <tabColor rgb="FF70AD47"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
@@ -1178,394 +1378,394 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col width="30" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="30" customWidth="1" style="48" min="1" max="1"/>
+    <col width="20" customWidth="1" style="48" min="2" max="4"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="16" t="inlineStr">
+    <row r="1" ht="16" customHeight="1" s="48">
+      <c r="A1" s="37" t="inlineStr">
         <is>
           <t>GAS / WATER / ELEKTRA DETAIL</t>
         </is>
       </c>
-      <c r="B1" s="2" t="n"/>
-      <c r="C1" s="2" t="n"/>
-      <c r="D1" s="2" t="n"/>
+      <c r="B1" s="38" t="n"/>
+      <c r="C1" s="38" t="n"/>
+      <c r="D1" s="34" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n"/>
-      <c r="B2" s="2" t="n"/>
-      <c r="C2" s="2" t="n"/>
-      <c r="D2" s="2" t="n"/>
+      <c r="A2" s="1" t="n"/>
+      <c r="B2" s="1" t="n"/>
+      <c r="C2" s="1" t="n"/>
+      <c r="D2" s="1" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="17" t="inlineStr">
+      <c r="A3" s="42" t="inlineStr">
         <is>
           <t>METERSTANDEN</t>
         </is>
       </c>
-      <c r="B3" s="2" t="n"/>
-      <c r="C3" s="2" t="n"/>
-      <c r="D3" s="2" t="n"/>
+      <c r="B3" s="38" t="n"/>
+      <c r="C3" s="38" t="n"/>
+      <c r="D3" s="34" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>Elektra (kWh) Begin *</t>
         </is>
       </c>
-      <c r="B4" s="18" t="n"/>
-      <c r="C4" s="2" t="n"/>
-      <c r="D4" s="2" t="n"/>
+      <c r="B4" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="C4" s="1" t="n"/>
+      <c r="D4" s="1" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>Elektra (kWh) Eind *</t>
         </is>
       </c>
-      <c r="B5" s="18" t="n"/>
-      <c r="C5" s="2" t="n"/>
-      <c r="D5" s="2" t="n"/>
+      <c r="B5" s="13" t="n">
+        <v>10850</v>
+      </c>
+      <c r="C5" s="1" t="n"/>
+      <c r="D5" s="1" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>Elektra (kWh) Verbruik (automatisch)</t>
         </is>
       </c>
-      <c r="B6" s="19">
-        <f>IF(AND(B4&lt;&gt;"",B5&lt;&gt;""),B5-B4,"")</f>
-        <v/>
-      </c>
-      <c r="C6" s="2" t="n"/>
-      <c r="D6" s="2" t="n"/>
+      <c r="B6" s="52" t="n">
+        <v>850</v>
+      </c>
+      <c r="C6" s="1" t="n"/>
+      <c r="D6" s="1" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>Gas (m³) Begin *</t>
         </is>
       </c>
-      <c r="B7" s="20" t="n"/>
-      <c r="C7" s="2" t="n"/>
-      <c r="D7" s="2" t="n"/>
+      <c r="B7" s="15" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C7" s="1" t="n"/>
+      <c r="D7" s="1" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="inlineStr">
+      <c r="A8" s="2" t="inlineStr">
         <is>
           <t>Gas (m³) Eind *</t>
         </is>
       </c>
-      <c r="B8" s="20" t="n"/>
-      <c r="C8" s="2" t="n"/>
-      <c r="D8" s="2" t="n"/>
+      <c r="B8" s="15" t="n">
+        <v>5120</v>
+      </c>
+      <c r="C8" s="1" t="n"/>
+      <c r="D8" s="1" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr">
         <is>
           <t>Gas (m³) Verbruik (automatisch)</t>
         </is>
       </c>
-      <c r="B9" s="21">
-        <f>IF(AND(B7&lt;&gt;"",B8&lt;&gt;""),B8-B7,"")</f>
-        <v/>
-      </c>
-      <c r="C9" s="2" t="n"/>
-      <c r="D9" s="2" t="n"/>
+      <c r="B9" s="53" t="n">
+        <v>120</v>
+      </c>
+      <c r="C9" s="1" t="n"/>
+      <c r="D9" s="1" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="n"/>
-      <c r="B10" s="2" t="n"/>
-      <c r="C10" s="2" t="n"/>
-      <c r="D10" s="2" t="n"/>
+      <c r="A10" s="1" t="n"/>
+      <c r="B10" s="1" t="n"/>
+      <c r="C10" s="1" t="n"/>
+      <c r="D10" s="1" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="17" t="inlineStr">
+      <c r="A11" s="42" t="inlineStr">
         <is>
           <t>KOSTENREGELS - Verbruik omzetten naar Euro's</t>
         </is>
       </c>
-      <c r="B11" s="2" t="n"/>
-      <c r="C11" s="2" t="n"/>
-      <c r="D11" s="2" t="n"/>
-    </row>
-    <row r="12" ht="30" customHeight="1">
-      <c r="A12" s="22" t="inlineStr">
+      <c r="B11" s="38" t="n"/>
+      <c r="C11" s="38" t="n"/>
+      <c r="D11" s="34" t="n"/>
+    </row>
+    <row r="12" ht="30" customHeight="1" s="48">
+      <c r="A12" s="54" t="inlineStr">
         <is>
           <t>💡 Vul hier de kosten in op basis van verbruik × tarief van energieleverancier. Voorbeelden staan hieronder (grijs). Verwijder voorbeelden en vul eigen regels in.</t>
         </is>
       </c>
-      <c r="B12" s="2" t="n"/>
-      <c r="C12" s="2" t="n"/>
-      <c r="D12" s="2" t="n"/>
-    </row>
-    <row r="13" ht="30" customHeight="1">
-      <c r="A13" s="23" t="inlineStr">
+      <c r="B12" s="38" t="n"/>
+      <c r="C12" s="38" t="n"/>
+      <c r="D12" s="34" t="n"/>
+    </row>
+    <row r="13" ht="30" customHeight="1" s="48">
+      <c r="A13" s="17" t="inlineStr">
         <is>
           <t>Omschrijving</t>
         </is>
       </c>
-      <c r="B13" s="23" t="inlineStr">
+      <c r="B13" s="17" t="inlineStr">
         <is>
           <t>Verbruik (kWh/m³) of Dagen</t>
         </is>
       </c>
-      <c r="C13" s="23" t="inlineStr">
+      <c r="C13" s="17" t="inlineStr">
         <is>
           <t>Tarief excl. BTW (€)</t>
         </is>
       </c>
-      <c r="D13" s="23" t="inlineStr">
+      <c r="D13" s="17" t="inlineStr">
         <is>
           <t>Kosten excl. BTW (€)</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="24" t="inlineStr">
+      <c r="A14" s="18" t="inlineStr">
         <is>
           <t>Elektra verbruik (zie meterstand)</t>
         </is>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="55">
         <f>KWh_verbruik</f>
         <v/>
       </c>
-      <c r="C14" s="26" t="n">
+      <c r="C14" s="56" t="n">
         <v>0.3</v>
       </c>
-      <c r="D14" s="26">
+      <c r="D14" s="56">
         <f>B14*C14</f>
         <v/>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="24" t="inlineStr">
+      <c r="A15" s="18" t="inlineStr">
         <is>
           <t>Gas verbruik (zie meterstand)</t>
         </is>
       </c>
-      <c r="B15" s="25">
+      <c r="B15" s="55">
         <f>Gas_verbruik</f>
         <v/>
       </c>
-      <c r="C15" s="26" t="n">
+      <c r="C15" s="56" t="n">
         <v>1.2</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="56">
         <f>B15*C15</f>
         <v/>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="24" t="inlineStr">
+      <c r="A16" s="18" t="inlineStr">
         <is>
           <t>Vaste levering elektra per dag</t>
         </is>
       </c>
-      <c r="B16" s="25">
-        <f>Algemeen!Aantal_dagen</f>
-        <v/>
-      </c>
-      <c r="C16" s="26" t="n">
+      <c r="B16" s="55">
+        <f>[0]!Aantal_dagen</f>
+        <v/>
+      </c>
+      <c r="C16" s="56" t="n">
         <v>0.5</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="56">
         <f>B16*C16</f>
         <v/>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="24" t="inlineStr">
+      <c r="A17" s="18" t="inlineStr">
         <is>
           <t>Vaste levering gas per dag</t>
         </is>
       </c>
-      <c r="B17" s="25">
-        <f>Algemeen!Aantal_dagen</f>
-        <v/>
-      </c>
-      <c r="C17" s="26" t="n">
+      <c r="B17" s="55">
+        <f>[0]!Aantal_dagen</f>
+        <v/>
+      </c>
+      <c r="C17" s="56" t="n">
         <v>0.45</v>
       </c>
-      <c r="D17" s="26">
+      <c r="D17" s="56">
         <f>B17*C17</f>
         <v/>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="24" t="inlineStr">
+      <c r="A18" s="18" t="inlineStr">
         <is>
           <t>Waterverbruik (geschat per dag)</t>
         </is>
       </c>
-      <c r="B18" s="25">
-        <f>Algemeen!Aantal_dagen</f>
-        <v/>
-      </c>
-      <c r="C18" s="26" t="n">
+      <c r="B18" s="55">
+        <f>[0]!Aantal_dagen</f>
+        <v/>
+      </c>
+      <c r="C18" s="56" t="n">
         <v>3.5</v>
       </c>
-      <c r="D18" s="26">
+      <c r="D18" s="56">
         <f>B18*C18</f>
         <v/>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="6" t="n"/>
-      <c r="B19" s="27" t="n"/>
-      <c r="C19" s="28" t="n"/>
-      <c r="D19" s="28" t="n"/>
+      <c r="A19" s="4" t="n"/>
+      <c r="B19" s="21" t="n"/>
+      <c r="C19" s="22" t="n"/>
+      <c r="D19" s="22" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="6" t="n"/>
-      <c r="B20" s="27" t="n"/>
-      <c r="C20" s="28" t="n"/>
-      <c r="D20" s="28" t="n"/>
+      <c r="A20" s="4" t="n"/>
+      <c r="B20" s="21" t="n"/>
+      <c r="C20" s="22" t="n"/>
+      <c r="D20" s="22" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="6" t="n"/>
-      <c r="B21" s="27" t="n"/>
-      <c r="C21" s="28" t="n"/>
-      <c r="D21" s="28" t="n"/>
+      <c r="A21" s="4" t="n"/>
+      <c r="B21" s="21" t="n"/>
+      <c r="C21" s="22" t="n"/>
+      <c r="D21" s="22" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="6" t="n"/>
-      <c r="B22" s="27" t="n"/>
-      <c r="C22" s="28" t="n"/>
-      <c r="D22" s="28" t="n"/>
+      <c r="A22" s="4" t="n"/>
+      <c r="B22" s="21" t="n"/>
+      <c r="C22" s="22" t="n"/>
+      <c r="D22" s="22" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="6" t="n"/>
-      <c r="B23" s="27" t="n"/>
-      <c r="C23" s="28" t="n"/>
-      <c r="D23" s="28" t="n"/>
+      <c r="A23" s="4" t="n"/>
+      <c r="B23" s="21" t="n"/>
+      <c r="C23" s="22" t="n"/>
+      <c r="D23" s="22" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="6" t="n"/>
-      <c r="B24" s="27" t="n"/>
-      <c r="C24" s="28" t="n"/>
-      <c r="D24" s="28" t="n"/>
+      <c r="A24" s="4" t="n"/>
+      <c r="B24" s="21" t="n"/>
+      <c r="C24" s="22" t="n"/>
+      <c r="D24" s="22" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="6" t="n"/>
-      <c r="B25" s="27" t="n"/>
-      <c r="C25" s="28" t="n"/>
-      <c r="D25" s="28" t="n"/>
+      <c r="A25" s="4" t="n"/>
+      <c r="B25" s="21" t="n"/>
+      <c r="C25" s="22" t="n"/>
+      <c r="D25" s="22" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="6" t="n"/>
-      <c r="B26" s="27" t="n"/>
-      <c r="C26" s="28" t="n"/>
-      <c r="D26" s="28" t="n"/>
+      <c r="A26" s="4" t="n"/>
+      <c r="B26" s="21" t="n"/>
+      <c r="C26" s="22" t="n"/>
+      <c r="D26" s="22" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="6" t="n"/>
-      <c r="B27" s="27" t="n"/>
-      <c r="C27" s="28" t="n"/>
-      <c r="D27" s="28" t="n"/>
+      <c r="A27" s="4" t="n"/>
+      <c r="B27" s="21" t="n"/>
+      <c r="C27" s="22" t="n"/>
+      <c r="D27" s="22" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="6" t="n"/>
-      <c r="B28" s="27" t="n"/>
-      <c r="C28" s="28" t="n"/>
-      <c r="D28" s="28" t="n"/>
+      <c r="A28" s="4" t="n"/>
+      <c r="B28" s="21" t="n"/>
+      <c r="C28" s="22" t="n"/>
+      <c r="D28" s="22" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="6" t="n"/>
-      <c r="B29" s="27" t="n"/>
-      <c r="C29" s="28" t="n"/>
-      <c r="D29" s="28" t="n"/>
+      <c r="A29" s="4" t="n"/>
+      <c r="B29" s="21" t="n"/>
+      <c r="C29" s="22" t="n"/>
+      <c r="D29" s="22" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="6" t="n"/>
-      <c r="B30" s="27" t="n"/>
-      <c r="C30" s="28" t="n"/>
-      <c r="D30" s="28" t="n"/>
+      <c r="A30" s="4" t="n"/>
+      <c r="B30" s="21" t="n"/>
+      <c r="C30" s="22" t="n"/>
+      <c r="D30" s="22" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="6" t="n"/>
-      <c r="B31" s="27" t="n"/>
-      <c r="C31" s="28" t="n"/>
-      <c r="D31" s="28" t="n"/>
+      <c r="A31" s="4" t="n"/>
+      <c r="B31" s="21" t="n"/>
+      <c r="C31" s="22" t="n"/>
+      <c r="D31" s="22" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="6" t="n"/>
-      <c r="B32" s="27" t="n"/>
-      <c r="C32" s="28" t="n"/>
-      <c r="D32" s="28" t="n"/>
+      <c r="A32" s="4" t="n"/>
+      <c r="B32" s="21" t="n"/>
+      <c r="C32" s="22" t="n"/>
+      <c r="D32" s="22" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="6" t="n"/>
-      <c r="B33" s="27" t="n"/>
-      <c r="C33" s="28" t="n"/>
-      <c r="D33" s="28" t="n"/>
+      <c r="A33" s="4" t="n"/>
+      <c r="B33" s="21" t="n"/>
+      <c r="C33" s="22" t="n"/>
+      <c r="D33" s="22" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" s="2" t="n"/>
-      <c r="B34" s="2" t="n"/>
-      <c r="C34" s="2" t="n"/>
-      <c r="D34" s="2" t="n"/>
+      <c r="A34" s="1" t="n"/>
+      <c r="B34" s="1" t="n"/>
+      <c r="C34" s="1" t="n"/>
+      <c r="D34" s="1" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="12" t="inlineStr">
+      <c r="A35" s="35" t="inlineStr">
         <is>
           <t>TOTALEN (automatisch berekend)</t>
         </is>
       </c>
-      <c r="B35" s="2" t="n"/>
-      <c r="C35" s="2" t="n"/>
-      <c r="D35" s="2" t="n"/>
+      <c r="B35" s="38" t="n"/>
+      <c r="C35" s="38" t="n"/>
+      <c r="D35" s="34" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="4" t="inlineStr">
+      <c r="A36" s="2" t="inlineStr">
         <is>
           <t>Totaal excl. BTW (automatisch)</t>
         </is>
       </c>
-      <c r="B36" s="11">
-        <f>SUM(D14:D34)</f>
-        <v/>
-      </c>
-      <c r="C36" s="2" t="n"/>
-      <c r="D36" s="2" t="n"/>
+      <c r="B36" s="50" t="n">
+        <v>484</v>
+      </c>
+      <c r="C36" s="1" t="n"/>
+      <c r="D36" s="1" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="4" t="inlineStr">
+      <c r="A37" s="2" t="inlineStr">
         <is>
           <t>BTW 21% (automatisch)</t>
         </is>
       </c>
-      <c r="B37" s="11">
-        <f>IF(B36="","",B36*0.21)</f>
-        <v/>
-      </c>
-      <c r="C37" s="2" t="n"/>
-      <c r="D37" s="2" t="n"/>
+      <c r="B37" s="50" t="n">
+        <v>101.64</v>
+      </c>
+      <c r="C37" s="1" t="n"/>
+      <c r="D37" s="1" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="29" t="inlineStr">
+      <c r="A38" s="23" t="inlineStr">
         <is>
           <t>Totaal incl. BTW (automatisch)</t>
         </is>
       </c>
-      <c r="B38" s="30">
-        <f>IF(B36="","",B36+B37)</f>
-        <v/>
-      </c>
-      <c r="C38" s="2" t="n"/>
-      <c r="D38" s="2" t="n"/>
+      <c r="B38" s="57" t="n">
+        <v>585.64</v>
+      </c>
+      <c r="C38" s="1" t="n"/>
+      <c r="D38" s="1" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1"/>
   <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A12:D12"/>
@@ -1580,7 +1780,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <tabColor rgb="00FFC000"/>
+    <tabColor rgb="FFFFC000"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
@@ -1588,95 +1788,99 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col width="35" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="35" customWidth="1" style="48" min="1" max="1"/>
+    <col width="20" customWidth="1" style="48" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="31" t="inlineStr">
+    <row r="1" ht="16" customHeight="1" s="48">
+      <c r="A1" s="58" t="inlineStr">
         <is>
           <t>SCHOONMAAK OVERZICHT</t>
         </is>
       </c>
-    </row>
-    <row r="2"/>
+      <c r="B1" s="34" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n"/>
+      <c r="B2" s="1" t="n"/>
+    </row>
     <row r="3">
-      <c r="A3" s="32" t="inlineStr">
+      <c r="A3" s="59" t="inlineStr">
         <is>
           <t>SCHOONMAAK GEGEVENS</t>
         </is>
       </c>
+      <c r="B3" s="34" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="33" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>Schoonmaak Pakket *</t>
         </is>
       </c>
-      <c r="B4" s="34">
-        <f>Algemeen!Schoonmaak_pakket_type</f>
+      <c r="B4" s="60">
+        <f>[0]!Schoonmaak_pakket_type</f>
         <v/>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="33" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>Inbegrepen Uren (automatisch)</t>
         </is>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="49">
         <f>IF(B4="Basis Schoonmaak",5,IF(B4="Intensief Schoonmaak",7,0))</f>
         <v/>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="33" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>Totaal Uren Gewerkt *</t>
         </is>
       </c>
-      <c r="B6" s="35" t="n"/>
+      <c r="B6" s="27" t="n">
+        <v>7.5</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="33" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>Extra Uren (automatisch)</t>
         </is>
       </c>
-      <c r="B7" s="36">
-        <f>IF(AND(B5&lt;&gt;"",B6&lt;&gt;""),MAX(0,B6-B5),"")</f>
-        <v/>
+      <c r="B7" s="61" t="n">
+        <v>2.5</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="33" t="inlineStr">
+      <c r="A8" s="2" t="inlineStr">
         <is>
           <t>Uurtarief *</t>
         </is>
       </c>
-      <c r="B8" s="37">
-        <f>Algemeen!Uurtarief_schoonmaak</f>
+      <c r="B8" s="62">
+        <f>[0]!Uurtarief_schoonmaak</f>
         <v/>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="38" t="inlineStr">
+      <c r="A9" s="23" t="inlineStr">
         <is>
           <t>Extra Schoonmaak Bedrag (automatisch)</t>
         </is>
       </c>
-      <c r="B9" s="30">
-        <f>IF(AND(B7&lt;&gt;"",B8&lt;&gt;""),B7*B8,"")</f>
-        <v/>
+      <c r="B9" s="57" t="n">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1"/>
   <mergeCells count="2">
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A1:B1"/>
@@ -1688,7 +1892,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <tabColor rgb="00C0504D"/>
+    <tabColor rgb="FFC0504D"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
@@ -1699,545 +1903,573 @@
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col width="50" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="50" customWidth="1" style="48" min="1" max="1"/>
+    <col width="12" customWidth="1" style="48" min="2" max="2"/>
+    <col width="20" customWidth="1" style="48" min="3" max="4"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="39" t="inlineStr">
+    <row r="1" ht="16" customHeight="1" s="48">
+      <c r="A1" s="63" t="inlineStr">
         <is>
           <t>SCHADEPOSTEN OVERZICHT</t>
         </is>
       </c>
-    </row>
-    <row r="2"/>
+      <c r="B1" s="38" t="n"/>
+      <c r="C1" s="38" t="n"/>
+      <c r="D1" s="34" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n"/>
+      <c r="B2" s="1" t="n"/>
+      <c r="C2" s="1" t="n"/>
+      <c r="D2" s="1" t="n"/>
+    </row>
     <row r="3">
-      <c r="A3" s="40" t="inlineStr">
+      <c r="A3" s="64" t="inlineStr">
         <is>
           <t>Vul hieronder alle schadeposten in. Bedrag wordt automatisch berekend (Aantal × Tarief).</t>
         </is>
       </c>
-    </row>
-    <row r="4"/>
-    <row r="5" ht="25" customHeight="1">
-      <c r="A5" s="41" t="inlineStr">
+      <c r="B3" s="1" t="n"/>
+      <c r="C3" s="1" t="n"/>
+      <c r="D3" s="1" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n"/>
+      <c r="B4" s="1" t="n"/>
+      <c r="C4" s="1" t="n"/>
+      <c r="D4" s="1" t="n"/>
+    </row>
+    <row r="5" ht="25" customHeight="1" s="48">
+      <c r="A5" s="65" t="inlineStr">
         <is>
           <t>Beschrijving</t>
         </is>
       </c>
-      <c r="B5" s="41" t="inlineStr">
+      <c r="B5" s="65" t="inlineStr">
         <is>
           <t>Aantal</t>
         </is>
       </c>
-      <c r="C5" s="41" t="inlineStr">
+      <c r="C5" s="65" t="inlineStr">
         <is>
           <t>Tarief excl. BTW</t>
         </is>
       </c>
-      <c r="D5" s="41" t="inlineStr">
+      <c r="D5" s="65" t="inlineStr">
         <is>
           <t>Bedrag excl. BTW</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="6" t="n"/>
-      <c r="B6" s="42" t="n"/>
-      <c r="C6" s="28" t="n"/>
-      <c r="D6" s="11">
+      <c r="A6" s="4" t="n"/>
+      <c r="B6" s="32" t="n"/>
+      <c r="C6" s="22" t="n"/>
+      <c r="D6" s="50">
         <f>IF(AND(B6&lt;&gt;"",C6&lt;&gt;""),B6*C6,"")</f>
         <v/>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="6" t="n"/>
-      <c r="B7" s="42" t="n"/>
-      <c r="C7" s="28" t="n"/>
-      <c r="D7" s="11">
+      <c r="A7" s="4" t="n"/>
+      <c r="B7" s="32" t="n"/>
+      <c r="C7" s="22" t="n"/>
+      <c r="D7" s="50">
         <f>IF(AND(B7&lt;&gt;"",C7&lt;&gt;""),B7*C7,"")</f>
         <v/>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="6" t="n"/>
-      <c r="B8" s="42" t="n"/>
-      <c r="C8" s="28" t="n"/>
-      <c r="D8" s="11">
+      <c r="A8" s="4" t="n"/>
+      <c r="B8" s="32" t="n"/>
+      <c r="C8" s="22" t="n"/>
+      <c r="D8" s="50">
         <f>IF(AND(B8&lt;&gt;"",C8&lt;&gt;""),B8*C8,"")</f>
         <v/>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="6" t="n"/>
-      <c r="B9" s="42" t="n"/>
-      <c r="C9" s="28" t="n"/>
-      <c r="D9" s="11">
+      <c r="A9" s="4" t="n"/>
+      <c r="B9" s="32" t="n"/>
+      <c r="C9" s="22" t="n"/>
+      <c r="D9" s="50">
         <f>IF(AND(B9&lt;&gt;"",C9&lt;&gt;""),B9*C9,"")</f>
         <v/>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="6" t="n"/>
-      <c r="B10" s="42" t="n"/>
-      <c r="C10" s="28" t="n"/>
-      <c r="D10" s="11">
+      <c r="A10" s="4" t="n"/>
+      <c r="B10" s="32" t="n"/>
+      <c r="C10" s="22" t="n"/>
+      <c r="D10" s="50">
         <f>IF(AND(B10&lt;&gt;"",C10&lt;&gt;""),B10*C10,"")</f>
         <v/>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="6" t="n"/>
-      <c r="B11" s="42" t="n"/>
-      <c r="C11" s="28" t="n"/>
-      <c r="D11" s="11">
+      <c r="A11" s="4" t="n"/>
+      <c r="B11" s="32" t="n"/>
+      <c r="C11" s="22" t="n"/>
+      <c r="D11" s="50">
         <f>IF(AND(B11&lt;&gt;"",C11&lt;&gt;""),B11*C11,"")</f>
         <v/>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="6" t="n"/>
-      <c r="B12" s="42" t="n"/>
-      <c r="C12" s="28" t="n"/>
-      <c r="D12" s="11">
+      <c r="A12" s="4" t="n"/>
+      <c r="B12" s="32" t="n"/>
+      <c r="C12" s="22" t="n"/>
+      <c r="D12" s="50">
         <f>IF(AND(B12&lt;&gt;"",C12&lt;&gt;""),B12*C12,"")</f>
         <v/>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="6" t="n"/>
-      <c r="B13" s="42" t="n"/>
-      <c r="C13" s="28" t="n"/>
-      <c r="D13" s="11">
+      <c r="A13" s="4" t="n"/>
+      <c r="B13" s="32" t="n"/>
+      <c r="C13" s="22" t="n"/>
+      <c r="D13" s="50">
         <f>IF(AND(B13&lt;&gt;"",C13&lt;&gt;""),B13*C13,"")</f>
         <v/>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="6" t="n"/>
-      <c r="B14" s="42" t="n"/>
-      <c r="C14" s="28" t="n"/>
-      <c r="D14" s="11">
+      <c r="A14" s="4" t="n"/>
+      <c r="B14" s="32" t="n"/>
+      <c r="C14" s="22" t="n"/>
+      <c r="D14" s="50">
         <f>IF(AND(B14&lt;&gt;"",C14&lt;&gt;""),B14*C14,"")</f>
         <v/>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="6" t="n"/>
-      <c r="B15" s="42" t="n"/>
-      <c r="C15" s="28" t="n"/>
-      <c r="D15" s="11">
+      <c r="A15" s="4" t="n"/>
+      <c r="B15" s="32" t="n"/>
+      <c r="C15" s="22" t="n"/>
+      <c r="D15" s="50">
         <f>IF(AND(B15&lt;&gt;"",C15&lt;&gt;""),B15*C15,"")</f>
         <v/>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="6" t="n"/>
-      <c r="B16" s="42" t="n"/>
-      <c r="C16" s="28" t="n"/>
-      <c r="D16" s="11">
+      <c r="A16" s="4" t="n"/>
+      <c r="B16" s="32" t="n"/>
+      <c r="C16" s="22" t="n"/>
+      <c r="D16" s="50">
         <f>IF(AND(B16&lt;&gt;"",C16&lt;&gt;""),B16*C16,"")</f>
         <v/>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="6" t="n"/>
-      <c r="B17" s="42" t="n"/>
-      <c r="C17" s="28" t="n"/>
-      <c r="D17" s="11">
+      <c r="A17" s="4" t="n"/>
+      <c r="B17" s="32" t="n"/>
+      <c r="C17" s="22" t="n"/>
+      <c r="D17" s="50">
         <f>IF(AND(B17&lt;&gt;"",C17&lt;&gt;""),B17*C17,"")</f>
         <v/>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="6" t="n"/>
-      <c r="B18" s="42" t="n"/>
-      <c r="C18" s="28" t="n"/>
-      <c r="D18" s="11">
+      <c r="A18" s="4" t="n"/>
+      <c r="B18" s="32" t="n"/>
+      <c r="C18" s="22" t="n"/>
+      <c r="D18" s="50">
         <f>IF(AND(B18&lt;&gt;"",C18&lt;&gt;""),B18*C18,"")</f>
         <v/>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="6" t="n"/>
-      <c r="B19" s="42" t="n"/>
-      <c r="C19" s="28" t="n"/>
-      <c r="D19" s="11">
+      <c r="A19" s="4" t="n"/>
+      <c r="B19" s="32" t="n"/>
+      <c r="C19" s="22" t="n"/>
+      <c r="D19" s="50">
         <f>IF(AND(B19&lt;&gt;"",C19&lt;&gt;""),B19*C19,"")</f>
         <v/>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="6" t="n"/>
-      <c r="B20" s="42" t="n"/>
-      <c r="C20" s="28" t="n"/>
-      <c r="D20" s="11">
+      <c r="A20" s="4" t="n"/>
+      <c r="B20" s="32" t="n"/>
+      <c r="C20" s="22" t="n"/>
+      <c r="D20" s="50">
         <f>IF(AND(B20&lt;&gt;"",C20&lt;&gt;""),B20*C20,"")</f>
         <v/>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="6" t="n"/>
-      <c r="B21" s="42" t="n"/>
-      <c r="C21" s="28" t="n"/>
-      <c r="D21" s="11">
+      <c r="A21" s="4" t="n"/>
+      <c r="B21" s="32" t="n"/>
+      <c r="C21" s="22" t="n"/>
+      <c r="D21" s="50">
         <f>IF(AND(B21&lt;&gt;"",C21&lt;&gt;""),B21*C21,"")</f>
         <v/>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="6" t="n"/>
-      <c r="B22" s="42" t="n"/>
-      <c r="C22" s="28" t="n"/>
-      <c r="D22" s="11">
+      <c r="A22" s="4" t="n"/>
+      <c r="B22" s="32" t="n"/>
+      <c r="C22" s="22" t="n"/>
+      <c r="D22" s="50">
         <f>IF(AND(B22&lt;&gt;"",C22&lt;&gt;""),B22*C22,"")</f>
         <v/>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="6" t="n"/>
-      <c r="B23" s="42" t="n"/>
-      <c r="C23" s="28" t="n"/>
-      <c r="D23" s="11">
+      <c r="A23" s="4" t="n"/>
+      <c r="B23" s="32" t="n"/>
+      <c r="C23" s="22" t="n"/>
+      <c r="D23" s="50">
         <f>IF(AND(B23&lt;&gt;"",C23&lt;&gt;""),B23*C23,"")</f>
         <v/>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="6" t="n"/>
-      <c r="B24" s="42" t="n"/>
-      <c r="C24" s="28" t="n"/>
-      <c r="D24" s="11">
+      <c r="A24" s="4" t="n"/>
+      <c r="B24" s="32" t="n"/>
+      <c r="C24" s="22" t="n"/>
+      <c r="D24" s="50">
         <f>IF(AND(B24&lt;&gt;"",C24&lt;&gt;""),B24*C24,"")</f>
         <v/>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="6" t="n"/>
-      <c r="B25" s="42" t="n"/>
-      <c r="C25" s="28" t="n"/>
-      <c r="D25" s="11">
+      <c r="A25" s="4" t="n"/>
+      <c r="B25" s="32" t="n"/>
+      <c r="C25" s="22" t="n"/>
+      <c r="D25" s="50">
         <f>IF(AND(B25&lt;&gt;"",C25&lt;&gt;""),B25*C25,"")</f>
         <v/>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="6" t="n"/>
-      <c r="B26" s="42" t="n"/>
-      <c r="C26" s="28" t="n"/>
-      <c r="D26" s="11">
+      <c r="A26" s="4" t="n"/>
+      <c r="B26" s="32" t="n"/>
+      <c r="C26" s="22" t="n"/>
+      <c r="D26" s="50">
         <f>IF(AND(B26&lt;&gt;"",C26&lt;&gt;""),B26*C26,"")</f>
         <v/>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="6" t="n"/>
-      <c r="B27" s="42" t="n"/>
-      <c r="C27" s="28" t="n"/>
-      <c r="D27" s="11">
+      <c r="A27" s="4" t="n"/>
+      <c r="B27" s="32" t="n"/>
+      <c r="C27" s="22" t="n"/>
+      <c r="D27" s="50">
         <f>IF(AND(B27&lt;&gt;"",C27&lt;&gt;""),B27*C27,"")</f>
         <v/>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="6" t="n"/>
-      <c r="B28" s="42" t="n"/>
-      <c r="C28" s="28" t="n"/>
-      <c r="D28" s="11">
+      <c r="A28" s="4" t="n"/>
+      <c r="B28" s="32" t="n"/>
+      <c r="C28" s="22" t="n"/>
+      <c r="D28" s="50">
         <f>IF(AND(B28&lt;&gt;"",C28&lt;&gt;""),B28*C28,"")</f>
         <v/>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="6" t="n"/>
-      <c r="B29" s="42" t="n"/>
-      <c r="C29" s="28" t="n"/>
-      <c r="D29" s="11">
+      <c r="A29" s="4" t="n"/>
+      <c r="B29" s="32" t="n"/>
+      <c r="C29" s="22" t="n"/>
+      <c r="D29" s="50">
         <f>IF(AND(B29&lt;&gt;"",C29&lt;&gt;""),B29*C29,"")</f>
         <v/>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="6" t="n"/>
-      <c r="B30" s="42" t="n"/>
-      <c r="C30" s="28" t="n"/>
-      <c r="D30" s="11">
+      <c r="A30" s="4" t="n"/>
+      <c r="B30" s="32" t="n"/>
+      <c r="C30" s="22" t="n"/>
+      <c r="D30" s="50">
         <f>IF(AND(B30&lt;&gt;"",C30&lt;&gt;""),B30*C30,"")</f>
         <v/>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="6" t="n"/>
-      <c r="B31" s="42" t="n"/>
-      <c r="C31" s="28" t="n"/>
-      <c r="D31" s="11">
+      <c r="A31" s="4" t="n"/>
+      <c r="B31" s="32" t="n"/>
+      <c r="C31" s="22" t="n"/>
+      <c r="D31" s="50">
         <f>IF(AND(B31&lt;&gt;"",C31&lt;&gt;""),B31*C31,"")</f>
         <v/>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="6" t="n"/>
-      <c r="B32" s="42" t="n"/>
-      <c r="C32" s="28" t="n"/>
-      <c r="D32" s="11">
+      <c r="A32" s="4" t="n"/>
+      <c r="B32" s="32" t="n"/>
+      <c r="C32" s="22" t="n"/>
+      <c r="D32" s="50">
         <f>IF(AND(B32&lt;&gt;"",C32&lt;&gt;""),B32*C32,"")</f>
         <v/>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="6" t="n"/>
-      <c r="B33" s="42" t="n"/>
-      <c r="C33" s="28" t="n"/>
-      <c r="D33" s="11">
+      <c r="A33" s="4" t="n"/>
+      <c r="B33" s="32" t="n"/>
+      <c r="C33" s="22" t="n"/>
+      <c r="D33" s="50">
         <f>IF(AND(B33&lt;&gt;"",C33&lt;&gt;""),B33*C33,"")</f>
         <v/>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="6" t="n"/>
-      <c r="B34" s="42" t="n"/>
-      <c r="C34" s="28" t="n"/>
-      <c r="D34" s="11">
+      <c r="A34" s="4" t="n"/>
+      <c r="B34" s="32" t="n"/>
+      <c r="C34" s="22" t="n"/>
+      <c r="D34" s="50">
         <f>IF(AND(B34&lt;&gt;"",C34&lt;&gt;""),B34*C34,"")</f>
         <v/>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="6" t="n"/>
-      <c r="B35" s="42" t="n"/>
-      <c r="C35" s="28" t="n"/>
-      <c r="D35" s="11">
+      <c r="A35" s="4" t="n"/>
+      <c r="B35" s="32" t="n"/>
+      <c r="C35" s="22" t="n"/>
+      <c r="D35" s="50">
         <f>IF(AND(B35&lt;&gt;"",C35&lt;&gt;""),B35*C35,"")</f>
         <v/>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="6" t="n"/>
-      <c r="B36" s="42" t="n"/>
-      <c r="C36" s="28" t="n"/>
-      <c r="D36" s="11">
+      <c r="A36" s="4" t="n"/>
+      <c r="B36" s="32" t="n"/>
+      <c r="C36" s="22" t="n"/>
+      <c r="D36" s="50">
         <f>IF(AND(B36&lt;&gt;"",C36&lt;&gt;""),B36*C36,"")</f>
         <v/>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="6" t="n"/>
-      <c r="B37" s="42" t="n"/>
-      <c r="C37" s="28" t="n"/>
-      <c r="D37" s="11">
+      <c r="A37" s="4" t="n"/>
+      <c r="B37" s="32" t="n"/>
+      <c r="C37" s="22" t="n"/>
+      <c r="D37" s="50">
         <f>IF(AND(B37&lt;&gt;"",C37&lt;&gt;""),B37*C37,"")</f>
         <v/>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="6" t="n"/>
-      <c r="B38" s="42" t="n"/>
-      <c r="C38" s="28" t="n"/>
-      <c r="D38" s="11">
+      <c r="A38" s="4" t="n"/>
+      <c r="B38" s="32" t="n"/>
+      <c r="C38" s="22" t="n"/>
+      <c r="D38" s="50">
         <f>IF(AND(B38&lt;&gt;"",C38&lt;&gt;""),B38*C38,"")</f>
         <v/>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="6" t="n"/>
-      <c r="B39" s="42" t="n"/>
-      <c r="C39" s="28" t="n"/>
-      <c r="D39" s="11">
+      <c r="A39" s="4" t="n"/>
+      <c r="B39" s="32" t="n"/>
+      <c r="C39" s="22" t="n"/>
+      <c r="D39" s="50">
         <f>IF(AND(B39&lt;&gt;"",C39&lt;&gt;""),B39*C39,"")</f>
         <v/>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="6" t="n"/>
-      <c r="B40" s="42" t="n"/>
-      <c r="C40" s="28" t="n"/>
-      <c r="D40" s="11">
+      <c r="A40" s="4" t="n"/>
+      <c r="B40" s="32" t="n"/>
+      <c r="C40" s="22" t="n"/>
+      <c r="D40" s="50">
         <f>IF(AND(B40&lt;&gt;"",C40&lt;&gt;""),B40*C40,"")</f>
         <v/>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="6" t="n"/>
-      <c r="B41" s="42" t="n"/>
-      <c r="C41" s="28" t="n"/>
-      <c r="D41" s="11">
+      <c r="A41" s="4" t="n"/>
+      <c r="B41" s="32" t="n"/>
+      <c r="C41" s="22" t="n"/>
+      <c r="D41" s="50">
         <f>IF(AND(B41&lt;&gt;"",C41&lt;&gt;""),B41*C41,"")</f>
         <v/>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="6" t="n"/>
-      <c r="B42" s="42" t="n"/>
-      <c r="C42" s="28" t="n"/>
-      <c r="D42" s="11">
+      <c r="A42" s="4" t="n"/>
+      <c r="B42" s="32" t="n"/>
+      <c r="C42" s="22" t="n"/>
+      <c r="D42" s="50">
         <f>IF(AND(B42&lt;&gt;"",C42&lt;&gt;""),B42*C42,"")</f>
         <v/>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="6" t="n"/>
-      <c r="B43" s="42" t="n"/>
-      <c r="C43" s="28" t="n"/>
-      <c r="D43" s="11">
+      <c r="A43" s="4" t="n"/>
+      <c r="B43" s="32" t="n"/>
+      <c r="C43" s="22" t="n"/>
+      <c r="D43" s="50">
         <f>IF(AND(B43&lt;&gt;"",C43&lt;&gt;""),B43*C43,"")</f>
         <v/>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="6" t="n"/>
-      <c r="B44" s="42" t="n"/>
-      <c r="C44" s="28" t="n"/>
-      <c r="D44" s="11">
+      <c r="A44" s="4" t="n"/>
+      <c r="B44" s="32" t="n"/>
+      <c r="C44" s="22" t="n"/>
+      <c r="D44" s="50">
         <f>IF(AND(B44&lt;&gt;"",C44&lt;&gt;""),B44*C44,"")</f>
         <v/>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="6" t="n"/>
-      <c r="B45" s="42" t="n"/>
-      <c r="C45" s="28" t="n"/>
-      <c r="D45" s="11">
+      <c r="A45" s="4" t="n"/>
+      <c r="B45" s="32" t="n"/>
+      <c r="C45" s="22" t="n"/>
+      <c r="D45" s="50">
         <f>IF(AND(B45&lt;&gt;"",C45&lt;&gt;""),B45*C45,"")</f>
         <v/>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="6" t="n"/>
-      <c r="B46" s="42" t="n"/>
-      <c r="C46" s="28" t="n"/>
-      <c r="D46" s="11">
+      <c r="A46" s="4" t="n"/>
+      <c r="B46" s="32" t="n"/>
+      <c r="C46" s="22" t="n"/>
+      <c r="D46" s="50">
         <f>IF(AND(B46&lt;&gt;"",C46&lt;&gt;""),B46*C46,"")</f>
         <v/>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="6" t="n"/>
-      <c r="B47" s="42" t="n"/>
-      <c r="C47" s="28" t="n"/>
-      <c r="D47" s="11">
+      <c r="A47" s="4" t="n"/>
+      <c r="B47" s="32" t="n"/>
+      <c r="C47" s="22" t="n"/>
+      <c r="D47" s="50">
         <f>IF(AND(B47&lt;&gt;"",C47&lt;&gt;""),B47*C47,"")</f>
         <v/>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="6" t="n"/>
-      <c r="B48" s="42" t="n"/>
-      <c r="C48" s="28" t="n"/>
-      <c r="D48" s="11">
+      <c r="A48" s="4" t="n"/>
+      <c r="B48" s="32" t="n"/>
+      <c r="C48" s="22" t="n"/>
+      <c r="D48" s="50">
         <f>IF(AND(B48&lt;&gt;"",C48&lt;&gt;""),B48*C48,"")</f>
         <v/>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="6" t="n"/>
-      <c r="B49" s="42" t="n"/>
-      <c r="C49" s="28" t="n"/>
-      <c r="D49" s="11">
+      <c r="A49" s="4" t="n"/>
+      <c r="B49" s="32" t="n"/>
+      <c r="C49" s="22" t="n"/>
+      <c r="D49" s="50">
         <f>IF(AND(B49&lt;&gt;"",C49&lt;&gt;""),B49*C49,"")</f>
         <v/>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="6" t="n"/>
-      <c r="B50" s="42" t="n"/>
-      <c r="C50" s="28" t="n"/>
-      <c r="D50" s="11">
+      <c r="A50" s="4" t="n"/>
+      <c r="B50" s="32" t="n"/>
+      <c r="C50" s="22" t="n"/>
+      <c r="D50" s="50">
         <f>IF(AND(B50&lt;&gt;"",C50&lt;&gt;""),B50*C50,"")</f>
         <v/>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="6" t="n"/>
-      <c r="B51" s="42" t="n"/>
-      <c r="C51" s="28" t="n"/>
-      <c r="D51" s="11">
+      <c r="A51" s="4" t="n"/>
+      <c r="B51" s="32" t="n"/>
+      <c r="C51" s="22" t="n"/>
+      <c r="D51" s="50">
         <f>IF(AND(B51&lt;&gt;"",C51&lt;&gt;""),B51*C51,"")</f>
         <v/>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="6" t="n"/>
-      <c r="B52" s="42" t="n"/>
-      <c r="C52" s="28" t="n"/>
-      <c r="D52" s="11">
+      <c r="A52" s="4" t="n"/>
+      <c r="B52" s="32" t="n"/>
+      <c r="C52" s="22" t="n"/>
+      <c r="D52" s="50">
         <f>IF(AND(B52&lt;&gt;"",C52&lt;&gt;""),B52*C52,"")</f>
         <v/>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="6" t="n"/>
-      <c r="B53" s="42" t="n"/>
-      <c r="C53" s="28" t="n"/>
-      <c r="D53" s="11">
+      <c r="A53" s="4" t="n"/>
+      <c r="B53" s="32" t="n"/>
+      <c r="C53" s="22" t="n"/>
+      <c r="D53" s="50">
         <f>IF(AND(B53&lt;&gt;"",C53&lt;&gt;""),B53*C53,"")</f>
         <v/>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="6" t="n"/>
-      <c r="B54" s="42" t="n"/>
-      <c r="C54" s="28" t="n"/>
-      <c r="D54" s="11">
+      <c r="A54" s="4" t="n"/>
+      <c r="B54" s="32" t="n"/>
+      <c r="C54" s="22" t="n"/>
+      <c r="D54" s="50">
         <f>IF(AND(B54&lt;&gt;"",C54&lt;&gt;""),B54*C54,"")</f>
         <v/>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="6" t="n"/>
-      <c r="B55" s="42" t="n"/>
-      <c r="C55" s="28" t="n"/>
-      <c r="D55" s="11">
+      <c r="A55" s="4" t="n"/>
+      <c r="B55" s="32" t="n"/>
+      <c r="C55" s="22" t="n"/>
+      <c r="D55" s="50">
         <f>IF(AND(B55&lt;&gt;"",C55&lt;&gt;""),B55*C55,"")</f>
         <v/>
       </c>
     </row>
-    <row r="56"/>
+    <row r="56">
+      <c r="A56" s="1" t="n"/>
+      <c r="B56" s="1" t="n"/>
+      <c r="C56" s="1" t="n"/>
+      <c r="D56" s="1" t="n"/>
+    </row>
     <row r="57">
-      <c r="A57" s="43" t="inlineStr">
+      <c r="A57" s="35" t="inlineStr">
         <is>
           <t>TOTALEN (automatisch berekend)</t>
         </is>
       </c>
+      <c r="B57" s="38" t="n"/>
+      <c r="C57" s="38" t="n"/>
+      <c r="D57" s="34" t="n"/>
     </row>
     <row r="58">
-      <c r="A58" s="33" t="inlineStr">
+      <c r="A58" s="2" t="inlineStr">
         <is>
           <t>Totaal Schade excl. BTW (automatisch)</t>
         </is>
       </c>
-      <c r="B58" s="11">
+      <c r="B58" s="50">
         <f>SUM(D6:D56)</f>
         <v/>
       </c>
+      <c r="C58" s="1" t="n"/>
+      <c r="D58" s="1" t="n"/>
     </row>
     <row r="59">
-      <c r="A59" s="33" t="inlineStr">
+      <c r="A59" s="2" t="inlineStr">
         <is>
           <t>BTW 21% (automatisch)</t>
         </is>
       </c>
-      <c r="B59" s="11">
+      <c r="B59" s="50">
         <f>IF(B58="","",B58*0.21)</f>
         <v/>
       </c>
+      <c r="C59" s="1" t="n"/>
+      <c r="D59" s="1" t="n"/>
     </row>
     <row r="60">
-      <c r="A60" s="38" t="inlineStr">
+      <c r="A60" s="23" t="inlineStr">
         <is>
           <t>Totaal Schade incl. BTW (automatisch)</t>
         </is>
       </c>
-      <c r="B60" s="30">
+      <c r="B60" s="57">
         <f>IF(B58="","",B58+B59)</f>
         <v/>
       </c>
+      <c r="C60" s="1" t="n"/>
+      <c r="D60" s="1" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1"/>
   <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A57:D57"/>
@@ -2245,271 +2477,4 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FD8216A3BCF59A4CAC1EDC9B65F03F94" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7a5dd83b0615c7ab65f6e497dc3f1a67">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7e7f2dcd-0c2b-4478-ad05-247cf739c5b2" xmlns:ns3="7c6541c9-858d-46cc-aee4-1fa681dc1bd6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b3083ab368e81f90f854d4b93d60013" ns2:_="" ns3:_="">
-    <xsd:import namespace="7e7f2dcd-0c2b-4478-ad05-247cf739c5b2"/>
-    <xsd:import namespace="7c6541c9-858d-46cc-aee4-1fa681dc1bd6"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="7e7f2dcd-0c2b-4478-ad05-247cf739c5b2" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="11" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="12" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="13" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="15" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="5bd66242-e0b1-4d5e-a424-ed2be647a714" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="17" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="18" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="21" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="22" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="7c6541c9-858d-46cc-aee4-1fa681dc1bd6" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="TaxCatchAll" ma:index="16" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{5de6d577-5e06-4df3-9e53-a11405c55b7c}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="7c6541c9-858d-46cc-aee4-1fa681dc1bd6">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithUsers" ma:index="19" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="20" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7e7f2dcd-0c2b-4478-ad05-247cf739c5b2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7c6541c9-858d-46cc-aee4-1fa681dc1bd6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBBA84A9-397E-4E12-BFFB-0436634DA3D5}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D15C3191-FDC9-4D92-8235-1C644D319F44}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B23D0D3-845A-442C-9FFB-B1B751F2D85B}"/>
 </file>
</xml_diff>

<commit_message>
updates aan the template
</commit_message>
<xml_diff>
--- a/input_template.xlsx
+++ b/input_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ryanrent.sharepoint.com/sites/RyanRent/Gedeelde documenten/General/01_RyanRent&amp;Co/Aljereau/Eindafrekening Generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="11_E0C8970C239286AD4E5E7607993545570676A730" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{517C8AEF-DE1B-7441-86F7-4B5EF1513CC3}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="11_E0C8970C239286AD4E5E7607993545570676A730" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2FE5AD0-CAD6-664E-AAD1-1F5527E0C522}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="780" windowWidth="17280" windowHeight="20280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Algemeen" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="96">
   <si>
     <t>RYANRENT EINDAFREKENING - BASISGEGEVENS</t>
   </si>
@@ -324,7 +324,7 @@
     <t>g</t>
   </si>
   <si>
-    <t>Intensief Schoonmaak</t>
+    <t>Basis Schoonmaak</t>
   </si>
   <si>
     <t>eneco</t>
@@ -339,12 +339,6 @@
     <t>Christa</t>
   </si>
   <si>
-    <t>pottn</t>
-  </si>
-  <si>
-    <t>kozijn</t>
-  </si>
-  <si>
     <t>Sophie van RyanRent</t>
   </si>
   <si>
@@ -375,46 +369,10 @@
     <t>Meerdere gaten in muren (herstel + schilderen)</t>
   </si>
   <si>
-    <t>Kapotte balkondeur inclusief slot</t>
-  </si>
-  <si>
-    <t>Beschadigde keukenkastjes (4 stuks)</t>
-  </si>
-  <si>
-    <t>Gebroken tegels badkamer + voegen</t>
-  </si>
-  <si>
-    <t>Brandschade op aanrechtblad</t>
-  </si>
-  <si>
-    <t>Kapotte wasmachine (tenant schade)</t>
-  </si>
-  <si>
-    <t>Schade aan gordijnen + rails (alle kamers)</t>
-  </si>
-  <si>
-    <t>Gebroken douchewand</t>
-  </si>
-  <si>
-    <t>Toegangspoort beschadigd</t>
-  </si>
-  <si>
-    <t>Waterlek schade plafond slaapkamer</t>
-  </si>
-  <si>
-    <t>Kapotte verlichting (lampen + armaturen)</t>
-  </si>
-  <si>
-    <t>Beschadigde radiator woonkamer</t>
-  </si>
-  <si>
-    <t>Verfschade op meerdere deuren</t>
-  </si>
-  <si>
-    <t>Kapotte vaatwasser (misbruik)</t>
-  </si>
-  <si>
-    <t>Hoge schade</t>
+    <t>underuse test</t>
+  </si>
+  <si>
+    <t>super water verbruik</t>
   </si>
 </sst>
 </file>
@@ -992,7 +950,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1019,7 +977,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1027,7 +985,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1035,7 +993,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1043,7 +1001,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1057,7 +1015,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1073,7 +1031,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1081,7 +1039,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1103,7 +1061,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -1111,7 +1069,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1181,7 +1139,7 @@
       </c>
       <c r="B29" s="5">
         <f>IF(B28="Basis Schoonmaak",5,IF(B28="Intensief Schoonmaak",7,""))</f>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1275,7 +1233,7 @@
       </c>
       <c r="B43" s="9">
         <f>[0]!Schade_totaal_incl</f>
-        <v>7580.65</v>
+        <v>1270.5</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -1284,7 +1242,7 @@
       </c>
       <c r="B44" s="9">
         <f>IF(Borg_gebruikt="","",Voorschot_borg-Borg_gebruikt)</f>
-        <v>-3580.6499999999996</v>
+        <v>2729.5</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -1293,7 +1251,7 @@
       </c>
       <c r="B45" s="9">
         <f>IF(Borg_gebruikt="","",MAX(0,Borg_gebruikt-Voorschot_borg))</f>
-        <v>3580.6499999999996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -1302,7 +1260,7 @@
       </c>
       <c r="B46" s="9">
         <f>IF([0]!GWE_totaal_incl="","",Voorschot_GWE-[0]!GWE_totaal_incl)</f>
-        <v>-1127.5500000000002</v>
+        <v>3293.79</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -1311,7 +1269,7 @@
       </c>
       <c r="B47" s="11">
         <f>IF(OR(Borg_terug="",GWE_meer_minder="",[0]!Extra_schoonmaak_bedrag=""),"",Borg_terug+GWE_meer_minder-[0]!Extra_schoonmaak_bedrag)</f>
-        <v>-5008.2</v>
+        <v>5923.29</v>
       </c>
     </row>
   </sheetData>
@@ -1347,7 +1305,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1385,7 +1343,7 @@
         <v>44</v>
       </c>
       <c r="B5" s="12">
-        <v>19500</v>
+        <v>15020</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1394,7 +1352,7 @@
       </c>
       <c r="B6" s="13">
         <f>IF(AND(B4&lt;&gt;"",B5&lt;&gt;""),B5-B4,"")</f>
-        <v>4500</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1410,7 +1368,7 @@
         <v>47</v>
       </c>
       <c r="B8" s="14">
-        <v>10200</v>
+        <v>8050</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1419,7 +1377,7 @@
       </c>
       <c r="B9" s="15">
         <f>IF(AND(B7&lt;&gt;"",B8&lt;&gt;""),B8-B7,"")</f>
-        <v>2200</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1458,14 +1416,14 @@
       </c>
       <c r="B14" s="18">
         <f>KWh_verbruik</f>
-        <v>4500</v>
+        <v>20</v>
       </c>
       <c r="C14" s="19">
         <v>0.3</v>
       </c>
       <c r="D14" s="19">
         <f>B14*C14</f>
-        <v>1350</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1474,14 +1432,14 @@
       </c>
       <c r="B15" s="18">
         <f>Gas_verbruik</f>
-        <v>2200</v>
+        <v>50</v>
       </c>
       <c r="C15" s="19">
         <v>1.2</v>
       </c>
       <c r="D15" s="19">
         <f>B15*C15</f>
-        <v>2640</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1530,10 +1488,19 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
+      <c r="A19" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="20">
+        <v>60</v>
+      </c>
+      <c r="C19" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="D19" s="7">
+        <f>B19*C19</f>
+        <v>270</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
@@ -1633,7 +1600,7 @@
       </c>
       <c r="B36" s="9">
         <f>SUM(D14:D34)</f>
-        <v>4155</v>
+        <v>501</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1642,7 +1609,7 @@
       </c>
       <c r="B37" s="9">
         <f>IF(B36="","",B36*0.21)</f>
-        <v>872.55</v>
+        <v>105.21</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1651,7 +1618,7 @@
       </c>
       <c r="B38" s="22">
         <f>IF(B36="","",B36+B37)</f>
-        <v>5027.55</v>
+        <v>606.21</v>
       </c>
     </row>
   </sheetData>
@@ -1675,7 +1642,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1702,7 +1669,7 @@
       </c>
       <c r="B4" s="23" t="str">
         <f>[0]!Schoonmaak_pakket</f>
-        <v>Intensief Schoonmaak</v>
+        <v>Basis Schoonmaak</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1711,7 +1678,7 @@
       </c>
       <c r="B5" s="5">
         <f>IF(B4="Basis Schoonmaak",5,IF(B4="Intensief Schoonmaak",7,""))</f>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1719,7 +1686,7 @@
         <v>66</v>
       </c>
       <c r="B6" s="24">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1728,7 +1695,7 @@
       </c>
       <c r="B7" s="25">
         <f>IF(AND(B5&lt;&gt;"",B6&lt;&gt;""),MAX(0,B6-B5),"")</f>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1746,7 +1713,7 @@
       </c>
       <c r="B9" s="22">
         <f>IF(AND(B7&lt;&gt;"",B8&lt;&gt;""),B7*B8,"")</f>
-        <v>300</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1766,8 +1733,8 @@
   <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C8:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1809,7 +1776,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B6" s="28">
         <v>1</v>
@@ -1824,7 +1791,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B7" s="28">
         <v>5</v>
@@ -1838,228 +1805,138 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B8" s="28">
-        <v>1</v>
-      </c>
-      <c r="C8" s="7">
-        <v>380</v>
-      </c>
-      <c r="D8" s="9">
-        <f t="shared" si="0"/>
-        <v>380</v>
+      <c r="A8" s="3"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B9" s="28">
-        <v>4</v>
-      </c>
-      <c r="C9" s="7">
-        <v>95</v>
-      </c>
-      <c r="D9" s="9">
-        <f t="shared" si="0"/>
-        <v>380</v>
+      <c r="A9" s="3"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B10" s="28">
-        <v>8</v>
-      </c>
-      <c r="C10" s="7">
-        <v>35</v>
-      </c>
-      <c r="D10" s="9">
-        <f t="shared" si="0"/>
-        <v>280</v>
+      <c r="A10" s="3"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B11" s="28">
-        <v>1</v>
-      </c>
-      <c r="C11" s="7">
-        <v>520</v>
-      </c>
-      <c r="D11" s="9">
-        <f t="shared" si="0"/>
-        <v>520</v>
+      <c r="A11" s="3"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B12" s="28">
-        <v>1</v>
-      </c>
-      <c r="C12" s="7">
-        <v>650</v>
-      </c>
-      <c r="D12" s="9">
-        <f t="shared" si="0"/>
-        <v>650</v>
+      <c r="A12" s="3"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B13" s="28">
-        <v>3</v>
-      </c>
-      <c r="C13" s="7">
-        <v>85</v>
-      </c>
-      <c r="D13" s="9">
-        <f t="shared" si="0"/>
-        <v>255</v>
+      <c r="A13" s="3"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B14" s="28">
-        <v>1</v>
-      </c>
-      <c r="C14" s="7">
-        <v>425</v>
-      </c>
-      <c r="D14" s="9">
-        <f t="shared" si="0"/>
-        <v>425</v>
+      <c r="A14" s="3"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B15" s="28">
-        <v>1</v>
-      </c>
-      <c r="C15" s="7">
-        <v>280</v>
-      </c>
-      <c r="D15" s="9">
-        <f t="shared" si="0"/>
-        <v>280</v>
+      <c r="A15" s="3"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B16" s="28">
-        <v>1</v>
-      </c>
-      <c r="C16" s="7">
-        <v>380</v>
-      </c>
-      <c r="D16" s="9">
-        <f t="shared" si="0"/>
-        <v>380</v>
+      <c r="A16" s="3"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B17" s="28">
-        <v>6</v>
-      </c>
-      <c r="C17" s="7">
-        <v>55</v>
-      </c>
-      <c r="D17" s="9">
-        <f t="shared" si="0"/>
-        <v>330</v>
+      <c r="A17" s="3"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B18" s="28">
-        <v>1</v>
-      </c>
-      <c r="C18" s="7">
-        <v>295</v>
-      </c>
-      <c r="D18" s="9">
-        <f t="shared" si="0"/>
-        <v>295</v>
+      <c r="A18" s="3"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B19" s="28">
-        <v>4</v>
-      </c>
-      <c r="C19" s="7">
-        <v>75</v>
-      </c>
-      <c r="D19" s="9">
-        <f t="shared" si="0"/>
-        <v>300</v>
+      <c r="A19" s="3"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B20" s="28">
-        <v>1</v>
-      </c>
-      <c r="C20" s="7">
-        <v>580</v>
-      </c>
-      <c r="D20" s="9">
-        <f t="shared" si="0"/>
-        <v>580</v>
+      <c r="A20" s="3"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B21" s="28">
-        <v>4</v>
-      </c>
-      <c r="C21" s="7">
-        <v>30</v>
-      </c>
-      <c r="D21" s="9">
-        <f t="shared" si="0"/>
-        <v>120</v>
+      <c r="A21" s="3"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B22" s="28">
-        <v>4</v>
-      </c>
-      <c r="C22" s="7">
-        <v>10</v>
-      </c>
-      <c r="D22" s="9">
-        <f t="shared" si="0"/>
-        <v>40</v>
+      <c r="A22" s="3"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -2373,7 +2250,7 @@
       </c>
       <c r="B58" s="9">
         <f>SUM(D6:D56)</f>
-        <v>6265</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -2382,7 +2259,7 @@
       </c>
       <c r="B59" s="9">
         <f>IF(B58="","",B58*0.21)</f>
-        <v>1315.6499999999999</v>
+        <v>220.5</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -2391,7 +2268,7 @@
       </c>
       <c r="B60" s="22">
         <f>IF(B58="","",B58+B59)</f>
-        <v>7580.65</v>
+        <v>1270.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Application fully functional and reports are properly generated
</commit_message>
<xml_diff>
--- a/input_template.xlsx
+++ b/input_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ryanrent.sharepoint.com/sites/RyanRent/Gedeelde documenten/General/01_RyanRent&amp;Co/Aljereau/Eindafrekening Generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="11_E0C8970C239286AD4E5E7607993545570676A730" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2FE5AD0-CAD6-664E-AAD1-1F5527E0C522}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_EF4826B6764B3C3690E2A462632658248408CB12" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1E742D0-E409-4644-BF03-E3BD1AF4A0E1}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4340" yWindow="760" windowWidth="30220" windowHeight="20240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Algemeen" sheetId="1" r:id="rId1"/>
@@ -20,49 +20,54 @@
   </sheets>
   <definedNames>
     <definedName name="Aantal_dagen">Algemeen!$B$19</definedName>
-    <definedName name="Borg_gebruikt">Algemeen!$B$43</definedName>
-    <definedName name="Borg_terug">Algemeen!$B$44</definedName>
+    <definedName name="Borg_gebruikt">Algemeen!$B$45</definedName>
+    <definedName name="Borg_terug">Algemeen!$B$46</definedName>
     <definedName name="Contactpersoon">Algemeen!$B$5</definedName>
-    <definedName name="Contractnummer">Algemeen!$B$33</definedName>
+    <definedName name="Contractnummer">Algemeen!$B$35</definedName>
     <definedName name="Email">Algemeen!$B$6</definedName>
-    <definedName name="Energie_leverancier">Algemeen!$B$32</definedName>
+    <definedName name="Energie_leverancier">Algemeen!$B$34</definedName>
     <definedName name="Extra_schoonmaak_bedrag">Schoonmaak!$B$9</definedName>
     <definedName name="Extra_uren">Schoonmaak!$B$7</definedName>
+    <definedName name="Extra_voorschot_bedrag">Algemeen!$B$26</definedName>
+    <definedName name="Extra_voorschot_gebruikt">Algemeen!$B$49</definedName>
+    <definedName name="Extra_voorschot_omschrijving">Algemeen!$B$27</definedName>
+    <definedName name="Extra_voorschot_restschade">Algemeen!$B$51</definedName>
+    <definedName name="Extra_voorschot_terug">Algemeen!$B$50</definedName>
     <definedName name="Gas_begin">GWE_Detail!$B$7</definedName>
     <definedName name="Gas_eind">GWE_Detail!$B$8</definedName>
     <definedName name="Gas_verbruik">GWE_Detail!$B$9</definedName>
     <definedName name="GWE_BTW">GWE_Detail!$B$37</definedName>
-    <definedName name="GWE_meer_minder">Algemeen!$B$46</definedName>
+    <definedName name="GWE_meer_minder">Algemeen!$B$48</definedName>
     <definedName name="GWE_totaal_excl">GWE_Detail!$B$36</definedName>
     <definedName name="GWE_totaal_incl">GWE_Detail!$B$38</definedName>
-    <definedName name="Inbegrepen_uren">Algemeen!$B$29</definedName>
+    <definedName name="Inbegrepen_uren">Algemeen!$B$31</definedName>
     <definedName name="Incheck_datum">Algemeen!$B$17</definedName>
     <definedName name="Klantnaam">Algemeen!$B$4</definedName>
     <definedName name="KWh_begin">GWE_Detail!$B$4</definedName>
     <definedName name="KWh_eind">GWE_Detail!$B$5</definedName>
     <definedName name="KWh_verbruik">GWE_Detail!$B$6</definedName>
-    <definedName name="Meterbeheerder">Algemeen!$B$31</definedName>
+    <definedName name="Meterbeheerder">Algemeen!$B$33</definedName>
     <definedName name="Object_adres">Algemeen!$B$10</definedName>
     <definedName name="Object_ID">Algemeen!$B$14</definedName>
     <definedName name="Overige_voorschotten">Algemeen!$B$25</definedName>
     <definedName name="Plaats">Algemeen!$B$13</definedName>
     <definedName name="Postcode">Algemeen!$B$12</definedName>
-    <definedName name="Restschade">Algemeen!$B$45</definedName>
-    <definedName name="RR_Factuurnummer">Algemeen!$B$40</definedName>
-    <definedName name="RR_Folder_link">Algemeen!$B$37</definedName>
-    <definedName name="RR_Inspecteur">Algemeen!$B$39</definedName>
-    <definedName name="RR_Klantnummer">Algemeen!$B$36</definedName>
-    <definedName name="RR_Projectleider">Algemeen!$B$38</definedName>
+    <definedName name="Restschade">Algemeen!$B$47</definedName>
+    <definedName name="RR_Factuurnummer">Algemeen!$B$42</definedName>
+    <definedName name="RR_Folder_link">Algemeen!$B$39</definedName>
+    <definedName name="RR_Inspecteur">Algemeen!$B$41</definedName>
+    <definedName name="RR_Klantnummer">Algemeen!$B$38</definedName>
+    <definedName name="RR_Projectleider">Algemeen!$B$40</definedName>
     <definedName name="Schade_BTW">Schade!$B$59</definedName>
     <definedName name="Schade_totaal_excl">Schade!$B$58</definedName>
     <definedName name="Schade_totaal_incl">Schade!$B$60</definedName>
-    <definedName name="Schoonmaak_pakket">Algemeen!$B$28</definedName>
+    <definedName name="Schoonmaak_pakket">Algemeen!$B$30</definedName>
     <definedName name="Telefoonnummer">Algemeen!$B$7</definedName>
-    <definedName name="Totaal_eindafrekening">Algemeen!$B$47</definedName>
+    <definedName name="Totaal_eindafrekening">Algemeen!$B$52</definedName>
     <definedName name="Totaal_uren_gew">Schoonmaak!$B$6</definedName>
     <definedName name="Uitcheck_datum">Algemeen!$B$18</definedName>
     <definedName name="Unit_nr">Algemeen!$B$11</definedName>
-    <definedName name="Uurtarief_schoonmaak">Algemeen!$B$30</definedName>
+    <definedName name="Uurtarief_schoonmaak">Algemeen!$B$32</definedName>
     <definedName name="Voorschot_borg">Algemeen!$B$22</definedName>
     <definedName name="Voorschot_GWE">Algemeen!$B$23</definedName>
     <definedName name="Voorschot_schoonmaak">Algemeen!$B$24</definedName>
@@ -85,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
   <si>
     <t>RYANRENT EINDAFREKENING - BASISGEGEVENS</t>
   </si>
@@ -150,6 +155,12 @@
     <t>Overige Voorschotten</t>
   </si>
   <si>
+    <t>Extra Voorschot Bedrag</t>
+  </si>
+  <si>
+    <t>Extra Voorschot Omschrijving</t>
+  </si>
+  <si>
     <t>CONTRACTGEGEVENS</t>
   </si>
   <si>
@@ -207,6 +218,15 @@
     <t>GWE Meer/Minder (automatisch)</t>
   </si>
   <si>
+    <t>Extra Voorschot Gebruikt *</t>
+  </si>
+  <si>
+    <t>Extra Voorschot Terug (automatisch)</t>
+  </si>
+  <si>
+    <t>Extra Voorschot Restschade (automatisch)</t>
+  </si>
+  <si>
     <t>Totaal Eindafrekening (automatisch)</t>
   </si>
   <si>
@@ -321,58 +341,7 @@
     <t>Totaal Schade incl. BTW (automatisch)</t>
   </si>
   <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>Basis Schoonmaak</t>
-  </si>
-  <si>
-    <t>eneco</t>
-  </si>
-  <si>
-    <t>vattenfall</t>
-  </si>
-  <si>
-    <t>Dion</t>
-  </si>
-  <si>
-    <t>Christa</t>
-  </si>
-  <si>
-    <t>Sophie van RyanRent</t>
-  </si>
-  <si>
-    <t>t.hendriksen@email.nl</t>
-  </si>
-  <si>
-    <t>06-12345678</t>
-  </si>
-  <si>
-    <t>Parkstraat 88</t>
-  </si>
-  <si>
-    <t>2000 XY</t>
-  </si>
-  <si>
-    <t>Utrecht</t>
-  </si>
-  <si>
-    <t>01-06-2024</t>
-  </si>
-  <si>
-    <t>30-11-2024</t>
-  </si>
-  <si>
-    <t>Grote schade aan vloerbedekking woonkamer</t>
-  </si>
-  <si>
-    <t>Meerdere gaten in muren (herstel + schilderen)</t>
-  </si>
-  <si>
-    <t>underuse test</t>
-  </si>
-  <si>
-    <t>super water verbruik</t>
+    <t>Testelooper</t>
   </si>
 </sst>
 </file>
@@ -383,7 +352,7 @@
     <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
     <numFmt numFmtId="165" formatCode="\€\ #,##0.00"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -461,14 +430,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -578,11 +539,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -639,10 +599,8 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -946,11 +904,11 @@
   <sheetPr>
     <tabColor rgb="FF1F4E78"/>
   </sheetPr>
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -977,32 +935,26 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>84</v>
-      </c>
+      <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="40" t="s">
-        <v>85</v>
-      </c>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="B7" s="3"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="29" t="s">
@@ -1014,41 +966,31 @@
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>87</v>
-      </c>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>78</v>
-      </c>
+      <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>88</v>
-      </c>
+      <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="3">
-        <v>999</v>
-      </c>
+      <c r="B14" s="3"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="29" t="s">
@@ -1060,25 +1002,21 @@
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>90</v>
-      </c>
+      <c r="B17" s="4"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>91</v>
-      </c>
+      <c r="B18" s="4"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="5" t="str">
         <f>IF(AND(B17&lt;&gt;"",B18&lt;&gt;""),B18-B17,"")</f>
-        <v>182</v>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -1091,158 +1029,132 @@
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="6">
-        <v>4000</v>
-      </c>
+      <c r="B22" s="6"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="6">
-        <v>3900</v>
-      </c>
+      <c r="B23" s="6"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="6">
-        <v>250</v>
-      </c>
+      <c r="B24" s="6"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B25" s="7">
-        <v>400</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="7">
+        <v>300</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" s="30"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>79</v>
-      </c>
+      <c r="B27" s="3"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="5">
-        <f>IF(B28="Basis Schoonmaak",5,IF(B28="Intensief Schoonmaak",7,""))</f>
-        <v>5</v>
-      </c>
+      <c r="B29" s="30"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="6">
-        <v>50</v>
-      </c>
+      <c r="B30" s="2"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>80</v>
+      <c r="B31" s="5" t="str">
+        <f>IF(B30="Basis Schoonmaak",5,IF(B30="Intensief Schoonmaak",7,""))</f>
+        <v/>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>81</v>
+      <c r="B32" s="6">
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="3">
-        <v>98746</v>
-      </c>
+      <c r="B33" s="3"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="3"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="B35" s="30"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+      <c r="A35" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="3">
-        <v>8847</v>
-      </c>
+      <c r="B35" s="3"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B37" s="3"/>
+      <c r="B37" s="30"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>82</v>
-      </c>
+      <c r="B38" s="3"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>83</v>
-      </c>
+      <c r="B39" s="3"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B40" s="3">
-        <v>8947483</v>
-      </c>
+      <c r="B40" s="3"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="3"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B42" s="30"/>
-      <c r="C42" s="8" t="s">
+      <c r="A42" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+      <c r="B42" s="3"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="B43" s="9">
-        <f>[0]!Schade_totaal_incl</f>
-        <v>1270.5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+      <c r="B44" s="30"/>
+      <c r="C44" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="B44" s="9">
-        <f>IF(Borg_gebruikt="","",Voorschot_borg-Borg_gebruikt)</f>
-        <v>2729.5</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -1250,7 +1162,7 @@
         <v>38</v>
       </c>
       <c r="B45" s="9">
-        <f>IF(Borg_gebruikt="","",MAX(0,Borg_gebruikt-Voorschot_borg))</f>
+        <f>[0]!Schade_totaal_incl</f>
         <v>0</v>
       </c>
     </row>
@@ -1259,40 +1171,80 @@
         <v>39</v>
       </c>
       <c r="B46" s="9">
+        <f>IF(Borg_gebruikt="","",Voorschot_borg-Borg_gebruikt)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B47" s="9">
+        <f>IF(Borg_gebruikt="","",MAX(0,Borg_gebruikt-Voorschot_borg))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" s="9" t="e">
         <f>IF([0]!GWE_totaal_incl="","",Voorschot_GWE-[0]!GWE_totaal_incl)</f>
-        <v>3293.79</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B47" s="11">
-        <f>IF(OR(Borg_terug="",GWE_meer_minder="",[0]!Extra_schoonmaak_bedrag=""),"",Borg_terug+GWE_meer_minder-[0]!Extra_schoonmaak_bedrag)</f>
-        <v>5923.29</v>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B49" s="6">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B50" s="9">
+        <f>IF(Extra_voorschot_bedrag=0,"",Extra_voorschot_bedrag-Extra_voorschot_gebruikt)</f>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B51" s="9">
+        <f>IF(Extra_voorschot_bedrag=0,"",MAX(0,Extra_voorschot_gebruikt-Extra_voorschot_bedrag))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B52" s="11" t="e">
+        <f>IF(OR(Borg_terug="",GWE_meer_minder="",[0]!Extra_schoonmaak_bedrag=""),"",Borg_terug+GWE_meer_minder-[0]!Extra_schoonmaak_bedrag+IF(Extra_voorschot_bedrag=0,0,Extra_voorschot_terug))</f>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A3:B3"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A44:B44"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" errorTitle="Ongeldige invoer" error="Kies 5_uur of 7_uur" sqref="B28" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>"Basis Schoonmaak,Intensief Schoonmaak"</formula1>
+    <dataValidation type="list" errorTitle="Ongeldige invoer" error="Kies geen, Basis Schoonmaak, of Intensief Schoonmaak" sqref="B30" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>"geen,Basis Schoonmaak,Intensief Schoonmaak"</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{4E977829-4C42-4C42-95B6-24DD5B4CCFE6}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1305,7 +1257,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16:B19"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1316,7 +1268,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -1324,7 +1276,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="35" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="30"/>
@@ -1332,57 +1284,49 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="12">
-        <v>15000</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="B4" s="12"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="12">
-        <v>15020</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="B5" s="12"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="13">
+        <v>50</v>
+      </c>
+      <c r="B6" s="13" t="str">
         <f>IF(AND(B4&lt;&gt;"",B5&lt;&gt;""),B5-B4,"")</f>
-        <v>20</v>
+        <v/>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="14">
-        <v>8000</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="B7" s="14"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="14">
-        <v>8050</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="B8" s="14"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="15">
+        <v>53</v>
+      </c>
+      <c r="B9" s="15" t="str">
         <f>IF(AND(B7&lt;&gt;"",B8&lt;&gt;""),B8-B7,"")</f>
-        <v>50</v>
+        <v/>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="35" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B11" s="30"/>
       <c r="C11" s="30"/>
@@ -1390,7 +1334,7 @@
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="34" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B12" s="30"/>
       <c r="C12" s="30"/>
@@ -1398,109 +1342,103 @@
     </row>
     <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" s="18">
+        <v>60</v>
+      </c>
+      <c r="B14" s="18" t="str">
         <f>KWh_verbruik</f>
-        <v>20</v>
+        <v/>
       </c>
       <c r="C14" s="19">
         <v>0.3</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="19" t="e">
         <f>B14*C14</f>
-        <v>6</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" s="18">
+        <v>61</v>
+      </c>
+      <c r="B15" s="18" t="str">
         <f>Gas_verbruik</f>
-        <v>50</v>
+        <v/>
       </c>
       <c r="C15" s="19">
         <v>1.2</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="19" t="e">
         <f>B15*C15</f>
-        <v>60</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" s="18">
-        <v>30</v>
+        <v>62</v>
+      </c>
+      <c r="B16" s="18" t="str">
+        <f>[0]!Aantal_dagen</f>
+        <v/>
       </c>
       <c r="C16" s="19">
         <v>0.5</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="19" t="e">
         <f>B16*C16</f>
-        <v>15</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B17" s="18">
-        <v>100</v>
+        <v>63</v>
+      </c>
+      <c r="B17" s="18" t="str">
+        <f>[0]!Aantal_dagen</f>
+        <v/>
       </c>
       <c r="C17" s="19">
         <v>0.45</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D17" s="19" t="e">
         <f>B17*C17</f>
-        <v>45</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="18">
-        <v>30</v>
+        <v>64</v>
+      </c>
+      <c r="B18" s="18" t="str">
+        <f>[0]!Aantal_dagen</f>
+        <v/>
       </c>
       <c r="C18" s="19">
         <v>3.5</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="19" t="e">
         <f>B18*C18</f>
-        <v>105</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B19" s="20">
-        <v>60</v>
-      </c>
-      <c r="C19" s="7">
-        <v>4.5</v>
-      </c>
-      <c r="D19" s="7">
-        <f>B19*C19</f>
-        <v>270</v>
-      </c>
+      <c r="A19" s="3"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
@@ -1588,7 +1526,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="31" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B35" s="30"/>
       <c r="C35" s="30"/>
@@ -1596,29 +1534,29 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B36" s="9">
+        <v>66</v>
+      </c>
+      <c r="B36" s="9" t="e">
         <f>SUM(D14:D34)</f>
-        <v>501</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B37" s="9">
+        <v>67</v>
+      </c>
+      <c r="B37" s="9" t="e">
         <f>IF(B36="","",B36*0.21)</f>
-        <v>105.21</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="B38" s="22">
+        <v>68</v>
+      </c>
+      <c r="B38" s="22" t="e">
         <f>IF(B36="","",B36+B37)</f>
-        <v>606.21</v>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
@@ -1642,7 +1580,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1653,54 +1591,52 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="37" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B1" s="30"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B3" s="30"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="23" t="str">
+        <v>24</v>
+      </c>
+      <c r="B4" s="23">
         <f>[0]!Schoonmaak_pakket</f>
-        <v>Basis Schoonmaak</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="5">
+        <v>25</v>
+      </c>
+      <c r="B5" s="5" t="str">
         <f>IF(B4="Basis Schoonmaak",5,IF(B4="Intensief Schoonmaak",7,""))</f>
-        <v>5</v>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="24">
-        <v>7</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="B6" s="24"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="25">
+        <v>72</v>
+      </c>
+      <c r="B7" s="25" t="str">
         <f>IF(AND(B5&lt;&gt;"",B6&lt;&gt;""),MAX(0,B6-B5),"")</f>
-        <v>2</v>
+        <v/>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B8" s="26">
         <f>[0]!Uurtarief_schoonmaak</f>
@@ -1709,11 +1645,11 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="22">
+        <v>74</v>
+      </c>
+      <c r="B9" s="22" t="str">
         <f>IF(AND(B7&lt;&gt;"",B8&lt;&gt;""),B7*B8,"")</f>
-        <v>100</v>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -1734,7 +1670,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C22" sqref="C8:C22"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1746,7 +1682,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="38" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -1754,7 +1690,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="39" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="30"/>
@@ -1762,46 +1698,34 @@
     </row>
     <row r="5" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" s="28">
-        <v>1</v>
-      </c>
-      <c r="C6" s="7">
-        <v>450</v>
-      </c>
-      <c r="D6" s="9">
+      <c r="A6" s="3"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="9" t="str">
         <f t="shared" ref="D6:D37" si="0">IF(AND(B6&lt;&gt;"",C6&lt;&gt;""),B6*C6,"")</f>
-        <v>450</v>
+        <v/>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B7" s="28">
-        <v>5</v>
-      </c>
-      <c r="C7" s="7">
-        <v>120</v>
-      </c>
-      <c r="D7" s="9">
-        <f t="shared" si="0"/>
-        <v>600</v>
+      <c r="A7" s="3"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2238,7 +2162,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="31" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B57" s="30"/>
       <c r="C57" s="30"/>
@@ -2246,29 +2170,29 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B58" s="9">
         <f>SUM(D6:D56)</f>
-        <v>1050</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B59" s="9">
         <f>IF(B58="","",B58*0.21)</f>
-        <v>220.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="21" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B60" s="22">
         <f>IF(B58="","",B58+B59)</f>
-        <v>1270.5</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2537,24 +2461,24 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0E34499-637D-4162-A805-7EFDC0DD1E38}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E525378-6FFF-426C-8B94-043C59AB313A}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="7e7f2dcd-0c2b-4478-ad05-247cf739c5b2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="7c6541c9-858d-46cc-aee4-1fa681dc1bd6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7e7f2dcd-0c2b-4478-ad05-247cf739c5b2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="7c6541c9-858d-46cc-aee4-1fa681dc1bd6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E4BE19B-BDEC-4623-9DE1-0A382A8AA918}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9A8D374-E72C-4F89-90F3-37EF1936E855}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
@@ -2562,7 +2486,7 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0714F983-1269-460F-8519-360A43876283}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7829040D-80C7-4350-BB6A-6BC478812A49}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>

</xml_diff>